<commit_message>
Implemented an assembly ticket lock but the difference between it and the c++ one was tiny so I discarded it. Gathered data on the ring buffer from stoker using perf and started gathering data from cube as I have discovered that it has 16 cores
</commit_message>
<xml_diff>
--- a/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
+++ b/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="84">
   <si>
     <t>Ring Buffer - Size (1000)= Doesn't matter since addition/removal is only done at the top of the queue</t>
   </si>
@@ -30,9 +30,6 @@
     <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) Locked</t>
   </si>
   <si>
-    <t>2 Core Intel CPU @ 2.80 GHz (D) Locked</t>
-  </si>
-  <si>
     <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) CAS lock</t>
   </si>
   <si>
@@ -85,6 +82,195 @@
   </si>
   <si>
     <t>Stoker CAS lock with no back off</t>
+  </si>
+  <si>
+    <t>task-clock</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>CPUs</t>
+  </si>
+  <si>
+    <t>utilized</t>
+  </si>
+  <si>
+    <t>context-switches</t>
+  </si>
+  <si>
+    <t>M/sec</t>
+  </si>
+  <si>
+    <t>CPU-migrations</t>
+  </si>
+  <si>
+    <t>page-faults</t>
+  </si>
+  <si>
+    <t>cycles</t>
+  </si>
+  <si>
+    <t>GHz</t>
+  </si>
+  <si>
+    <t>[83.31%]</t>
+  </si>
+  <si>
+    <t>stalled-cycles-frontend</t>
+  </si>
+  <si>
+    <t>frontend</t>
+  </si>
+  <si>
+    <t>idle</t>
+  </si>
+  <si>
+    <t>[83.28%]</t>
+  </si>
+  <si>
+    <t>stalled-cycles-backend</t>
+  </si>
+  <si>
+    <t>backend</t>
+  </si>
+  <si>
+    <t>[66.63%]</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>insns</t>
+  </si>
+  <si>
+    <t>per</t>
+  </si>
+  <si>
+    <t>cycle</t>
+  </si>
+  <si>
+    <t>stalled</t>
+  </si>
+  <si>
+    <t>insn</t>
+  </si>
+  <si>
+    <t>[83.37%]</t>
+  </si>
+  <si>
+    <t>branches</t>
+  </si>
+  <si>
+    <t>[83.41%]</t>
+  </si>
+  <si>
+    <t>branch-misses</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>[83.44%]</t>
+  </si>
+  <si>
+    <t>Stoker Locked</t>
+  </si>
+  <si>
+    <t>[83.35%]</t>
+  </si>
+  <si>
+    <t>[82.45%]</t>
+  </si>
+  <si>
+    <t>Stoker CAS lock</t>
+  </si>
+  <si>
+    <t>Stoker TAS lock</t>
+  </si>
+  <si>
+    <t>Stoker TTAS lock</t>
+  </si>
+  <si>
+    <t>Stoker Ticket lock</t>
+  </si>
+  <si>
+    <t>[83.62%]</t>
+  </si>
+  <si>
+    <t>[66.23%]</t>
+  </si>
+  <si>
+    <t>[83.83%]</t>
+  </si>
+  <si>
+    <t>[83.34%]</t>
+  </si>
+  <si>
+    <t>[84.45%]</t>
+  </si>
+  <si>
+    <t>[83.48%]</t>
+  </si>
+  <si>
+    <t>[83.02%]</t>
+  </si>
+  <si>
+    <t>[66.40%]</t>
+  </si>
+  <si>
+    <t>[83.68%]</t>
+  </si>
+  <si>
+    <t>[83.71%]</t>
+  </si>
+  <si>
+    <t>[66.49%]</t>
+  </si>
+  <si>
+    <t>[83.27%]</t>
+  </si>
+  <si>
+    <t>[83.38%]</t>
+  </si>
+  <si>
+    <t>[83.46%]</t>
+  </si>
+  <si>
+    <t>[83.40%]</t>
+  </si>
+  <si>
+    <t>[83.17%]</t>
+  </si>
+  <si>
+    <t>[67.30%]</t>
+  </si>
+  <si>
+    <t>[83.85%]</t>
+  </si>
+  <si>
+    <t>[83.96%]</t>
+  </si>
+  <si>
+    <t>16 Core Intel CPU @ 2.27 GHz (E ) CAS</t>
+  </si>
+  <si>
+    <t>16 Core Intel CPU @ 2.27 GHz (E ) Ticket</t>
+  </si>
+  <si>
+    <t>16 Core Intel CPU @ 2.27 GHz (E ) TAS</t>
+  </si>
+  <si>
+    <t>16 Core Intel CPU @ 2.27 GHz (E ) TTAS</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 2.80 GHz (D Spoon) Locked</t>
+  </si>
+  <si>
+    <t>16 Core Intel CPU @ 2.27 GHz (E Cube ) Locked</t>
   </si>
 </sst>
 </file>
@@ -120,11 +306,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,19 +614,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A9:I34"/>
+  <dimension ref="A4:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.140625" customWidth="1"/>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>6813876</v>
+      </c>
+      <c r="C4">
+        <v>13561445</v>
+      </c>
+      <c r="D4">
+        <v>10716292</v>
+      </c>
+      <c r="E4">
+        <v>9389905</v>
+      </c>
+      <c r="F4">
+        <v>11458014</v>
+      </c>
+      <c r="G4">
+        <v>6445226</v>
+      </c>
+      <c r="H4">
+        <v>10594142</v>
+      </c>
+      <c r="I4">
+        <v>5268522</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>6813876</v>
+      </c>
+    </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
@@ -509,7 +729,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>5642544</v>
@@ -538,7 +758,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>6163242</v>
@@ -567,7 +787,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>4910844</v>
@@ -596,7 +816,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>4235748</v>
@@ -654,7 +874,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>9771618</v>
@@ -683,7 +903,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>14077775</v>
@@ -712,7 +932,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>10644755</v>
@@ -741,7 +961,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>10604337</v>
@@ -770,7 +990,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21">
         <v>1321542</v>
@@ -799,7 +1019,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22">
         <v>1249352</v>
@@ -828,7 +1048,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23">
         <v>1401147</v>
@@ -857,7 +1077,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24">
         <v>1303082</v>
@@ -886,7 +1106,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>1191029</v>
@@ -915,7 +1135,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="B26">
         <v>3421422</v>
@@ -944,7 +1164,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27">
         <v>2642745</v>
@@ -973,7 +1193,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>3960868</v>
@@ -1002,7 +1222,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29">
         <v>2581570</v>
@@ -1031,7 +1251,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30">
         <v>2560144</v>
@@ -1058,33 +1278,1376 @@
         <v>2445529</v>
       </c>
     </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31">
+        <v>6813876</v>
+      </c>
+      <c r="C31">
+        <v>13561445</v>
+      </c>
+      <c r="D31">
+        <v>10716292</v>
+      </c>
+      <c r="E31">
+        <v>9389905</v>
+      </c>
+      <c r="F31">
+        <v>11458014</v>
+      </c>
+      <c r="G31">
+        <v>6445226</v>
+      </c>
+      <c r="H31">
+        <v>10594142</v>
+      </c>
+      <c r="I31">
+        <v>5268522</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32">
+        <v>6003533</v>
+      </c>
+      <c r="C32">
+        <v>7571208</v>
+      </c>
+      <c r="D32">
+        <v>5799059</v>
+      </c>
+      <c r="E32">
+        <v>7543689</v>
+      </c>
+      <c r="F32">
+        <v>5793887</v>
+      </c>
+      <c r="G32">
+        <v>7527437</v>
+      </c>
+      <c r="H32">
+        <v>6002122</v>
+      </c>
+      <c r="I32">
+        <v>5780359</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33">
+        <v>7482005</v>
+      </c>
+      <c r="C33">
+        <v>412</v>
+      </c>
+      <c r="D33">
+        <v>190</v>
+      </c>
+      <c r="E33">
+        <v>208</v>
+      </c>
+      <c r="F33">
+        <v>295</v>
+      </c>
+      <c r="G33">
+        <v>36</v>
+      </c>
+      <c r="H33">
+        <v>505</v>
+      </c>
+      <c r="I33">
+        <v>215</v>
+      </c>
+    </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34">
+        <v>6255918</v>
+      </c>
+      <c r="C34">
+        <v>9239428</v>
+      </c>
+      <c r="D34">
+        <v>1671904</v>
+      </c>
+      <c r="E34">
+        <v>1033345</v>
+      </c>
+      <c r="F34">
+        <v>1092124</v>
+      </c>
+      <c r="G34">
+        <v>1006588</v>
+      </c>
+      <c r="H34">
+        <v>792270</v>
+      </c>
+      <c r="I34">
+        <v>194233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35">
+        <v>6101158</v>
+      </c>
+      <c r="C35">
+        <v>6096248</v>
+      </c>
+      <c r="D35">
+        <v>6564101</v>
+      </c>
+      <c r="E35">
+        <v>6351205</v>
+      </c>
+      <c r="F35">
+        <v>6084325</v>
+      </c>
+      <c r="G35">
+        <v>5934312</v>
+      </c>
+      <c r="H35">
+        <v>6006657</v>
+      </c>
+      <c r="I35">
+        <v>6067944</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>5239892</v>
+      </c>
+      <c r="C37">
+        <v>4292418</v>
+      </c>
+      <c r="D37">
+        <v>4107789</v>
+      </c>
+      <c r="E37">
+        <v>2487322</v>
+      </c>
+      <c r="F37">
+        <v>1586250</v>
+      </c>
+      <c r="G37">
+        <v>217490</v>
+      </c>
+      <c r="H37">
+        <v>118332</v>
+      </c>
+      <c r="I37">
+        <v>262630</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40">
+        <v>154528.90856700001</v>
+      </c>
+      <c r="C40" t="s">
         <v>21</v>
       </c>
-      <c r="B34">
-        <v>5239892</v>
-      </c>
-      <c r="C34">
-        <v>4292418</v>
-      </c>
-      <c r="D34">
-        <v>4107789</v>
-      </c>
-      <c r="E34">
-        <v>2487322</v>
-      </c>
-      <c r="F34">
-        <v>1586250</v>
-      </c>
-      <c r="G34">
-        <v>217490</v>
-      </c>
-      <c r="H34">
-        <v>118332</v>
-      </c>
-      <c r="I34">
-        <v>262630</v>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40">
+        <v>19.286999999999999</v>
+      </c>
+      <c r="F40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>125793</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41">
+        <v>1E-3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>895</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>4880</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>309567365952</v>
+      </c>
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44">
+        <v>2.0030000000000001</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>292660249898</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0.94540000000000002</v>
+      </c>
+      <c r="F45" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" t="s">
+        <v>34</v>
+      </c>
+      <c r="I45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>188147577898</v>
+      </c>
+      <c r="C46" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.60780000000000001</v>
+      </c>
+      <c r="F46" t="s">
+        <v>37</v>
+      </c>
+      <c r="G46" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" t="s">
+        <v>34</v>
+      </c>
+      <c r="I46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>30388998863</v>
+      </c>
+      <c r="C47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47">
+        <v>0.1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" t="s">
+        <v>41</v>
+      </c>
+      <c r="H47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" t="s">
+        <v>41</v>
+      </c>
+      <c r="G48" t="s">
+        <v>44</v>
+      </c>
+      <c r="H48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
+        <v>10528527003</v>
+      </c>
+      <c r="C49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49">
+        <v>68.132999999999996</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <v>9315830</v>
+      </c>
+      <c r="C50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="3">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>49</v>
+      </c>
+      <c r="G50" t="s">
+        <v>50</v>
+      </c>
+      <c r="H50" t="s">
+        <v>46</v>
+      </c>
+      <c r="I50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>10695.285760999999</v>
+      </c>
+      <c r="C53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53">
+        <v>1.329</v>
+      </c>
+      <c r="F53" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="2">
+        <v>309495</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E54">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="2">
+        <v>5967</v>
+      </c>
+      <c r="C55" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
+      <c r="E55">
+        <v>1E-3</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="2">
+        <v>6308</v>
+      </c>
+      <c r="C56" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56">
+        <v>1E-3</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
+        <v>11270458403</v>
+      </c>
+      <c r="C57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57">
+        <v>1.054</v>
+      </c>
+      <c r="F57" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="2">
+        <v>6848111760</v>
+      </c>
+      <c r="C58" t="s">
+        <v>32</v>
+      </c>
+      <c r="D58" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0.60760000000000003</v>
+      </c>
+      <c r="F58" t="s">
+        <v>33</v>
+      </c>
+      <c r="G58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H58" t="s">
+        <v>34</v>
+      </c>
+      <c r="I58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="2">
+        <v>4364938024</v>
+      </c>
+      <c r="C59" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0.38729999999999998</v>
+      </c>
+      <c r="F59" t="s">
+        <v>37</v>
+      </c>
+      <c r="G59" t="s">
+        <v>29</v>
+      </c>
+      <c r="H59" t="s">
+        <v>34</v>
+      </c>
+      <c r="I59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="2">
+        <v>9661845211</v>
+      </c>
+      <c r="C60" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60">
+        <v>0.86</v>
+      </c>
+      <c r="F60" t="s">
+        <v>40</v>
+      </c>
+      <c r="G60" t="s">
+        <v>41</v>
+      </c>
+      <c r="H60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61">
+        <v>0.71</v>
+      </c>
+      <c r="D61" t="s">
+        <v>43</v>
+      </c>
+      <c r="E61" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" t="s">
+        <v>41</v>
+      </c>
+      <c r="G61" t="s">
+        <v>44</v>
+      </c>
+      <c r="H61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="2">
+        <v>1920524089</v>
+      </c>
+      <c r="C62" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62">
+        <v>179.56700000000001</v>
+      </c>
+      <c r="F62" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="2">
+        <v>7340566</v>
+      </c>
+      <c r="C63" t="s">
+        <v>48</v>
+      </c>
+      <c r="D63" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="3">
+        <v>3.8E-3</v>
+      </c>
+      <c r="F63" t="s">
+        <v>49</v>
+      </c>
+      <c r="G63" t="s">
+        <v>50</v>
+      </c>
+      <c r="H63" t="s">
+        <v>46</v>
+      </c>
+      <c r="I63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>8045.4323169999998</v>
+      </c>
+      <c r="C66" t="s">
+        <v>21</v>
+      </c>
+      <c r="D66" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="F66" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="2">
+        <v>526</v>
+      </c>
+      <c r="C67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="2">
+        <v>273</v>
+      </c>
+      <c r="C68" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="2">
+        <v>3759</v>
+      </c>
+      <c r="C69" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="2">
+        <v>12801950363</v>
+      </c>
+      <c r="C70" t="s">
+        <v>29</v>
+      </c>
+      <c r="D70" t="s">
+        <v>22</v>
+      </c>
+      <c r="E70">
+        <v>1.591</v>
+      </c>
+      <c r="F70" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="2">
+        <v>7550260810</v>
+      </c>
+      <c r="C71" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0.58979999999999999</v>
+      </c>
+      <c r="F71" t="s">
+        <v>33</v>
+      </c>
+      <c r="G71" t="s">
+        <v>29</v>
+      </c>
+      <c r="H71" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="2">
+        <v>4569939952</v>
+      </c>
+      <c r="C72" t="s">
+        <v>36</v>
+      </c>
+      <c r="D72" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="3">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="F72" t="s">
+        <v>37</v>
+      </c>
+      <c r="G72" t="s">
+        <v>29</v>
+      </c>
+      <c r="H72" t="s">
+        <v>34</v>
+      </c>
+      <c r="I72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="2">
+        <v>13025703849</v>
+      </c>
+      <c r="C73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73">
+        <v>1.02</v>
+      </c>
+      <c r="F73" t="s">
+        <v>40</v>
+      </c>
+      <c r="G73" t="s">
+        <v>41</v>
+      </c>
+      <c r="H73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D74" t="s">
+        <v>43</v>
+      </c>
+      <c r="E74" t="s">
+        <v>29</v>
+      </c>
+      <c r="F74" t="s">
+        <v>41</v>
+      </c>
+      <c r="G74" t="s">
+        <v>44</v>
+      </c>
+      <c r="H74" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="2">
+        <v>2506811383</v>
+      </c>
+      <c r="C75" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" t="s">
+        <v>22</v>
+      </c>
+      <c r="E75">
+        <v>311.58199999999999</v>
+      </c>
+      <c r="F75" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
+        <v>236508</v>
+      </c>
+      <c r="C76" t="s">
+        <v>48</v>
+      </c>
+      <c r="D76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F76" t="s">
+        <v>49</v>
+      </c>
+      <c r="G76" t="s">
+        <v>50</v>
+      </c>
+      <c r="H76" t="s">
+        <v>46</v>
+      </c>
+      <c r="I76" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>188185.89483400001</v>
+      </c>
+      <c r="C79" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79">
+        <v>23.465</v>
+      </c>
+      <c r="F79" t="s">
+        <v>23</v>
+      </c>
+      <c r="G79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="2">
+        <v>4235</v>
+      </c>
+      <c r="C80" t="s">
+        <v>25</v>
+      </c>
+      <c r="D80" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="2">
+        <v>329</v>
+      </c>
+      <c r="C81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="2">
+        <v>2388</v>
+      </c>
+      <c r="C82" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="2">
+        <v>391423099860</v>
+      </c>
+      <c r="C83" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83">
+        <v>2.08</v>
+      </c>
+      <c r="F83" t="s">
+        <v>30</v>
+      </c>
+      <c r="G83" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="2">
+        <v>387870592065</v>
+      </c>
+      <c r="C84" t="s">
+        <v>32</v>
+      </c>
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="3">
+        <v>0.9909</v>
+      </c>
+      <c r="F84" t="s">
+        <v>33</v>
+      </c>
+      <c r="G84" t="s">
+        <v>29</v>
+      </c>
+      <c r="H84" t="s">
+        <v>34</v>
+      </c>
+      <c r="I84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="2">
+        <v>327940949960</v>
+      </c>
+      <c r="C85" t="s">
+        <v>36</v>
+      </c>
+      <c r="D85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" s="3">
+        <v>0.83779999999999999</v>
+      </c>
+      <c r="F85" t="s">
+        <v>37</v>
+      </c>
+      <c r="G85" t="s">
+        <v>29</v>
+      </c>
+      <c r="H85" t="s">
+        <v>34</v>
+      </c>
+      <c r="I85" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="2">
+        <v>9389575924</v>
+      </c>
+      <c r="C86" t="s">
+        <v>39</v>
+      </c>
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86">
+        <v>0.02</v>
+      </c>
+      <c r="F86" t="s">
+        <v>40</v>
+      </c>
+      <c r="G86" t="s">
+        <v>41</v>
+      </c>
+      <c r="H86" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87">
+        <v>41.31</v>
+      </c>
+      <c r="D87" t="s">
+        <v>43</v>
+      </c>
+      <c r="E87" t="s">
+        <v>29</v>
+      </c>
+      <c r="F87" t="s">
+        <v>41</v>
+      </c>
+      <c r="G87" t="s">
+        <v>44</v>
+      </c>
+      <c r="H87" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="2">
+        <v>1651093111</v>
+      </c>
+      <c r="C88" t="s">
+        <v>46</v>
+      </c>
+      <c r="D88" t="s">
+        <v>22</v>
+      </c>
+      <c r="E88">
+        <v>8.7739999999999991</v>
+      </c>
+      <c r="F88" t="s">
+        <v>26</v>
+      </c>
+      <c r="G88" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="2">
+        <v>2658981</v>
+      </c>
+      <c r="C89" t="s">
+        <v>48</v>
+      </c>
+      <c r="D89" t="s">
+        <v>22</v>
+      </c>
+      <c r="E89" s="3">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="F89" t="s">
+        <v>49</v>
+      </c>
+      <c r="G89" t="s">
+        <v>50</v>
+      </c>
+      <c r="H89" t="s">
+        <v>46</v>
+      </c>
+      <c r="I89" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>1076.193186</v>
+      </c>
+      <c r="C92" t="s">
+        <v>21</v>
+      </c>
+      <c r="D92" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F92" t="s">
+        <v>23</v>
+      </c>
+      <c r="G92" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>503</v>
+      </c>
+      <c r="C93" t="s">
+        <v>25</v>
+      </c>
+      <c r="D93" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>257</v>
+      </c>
+      <c r="C94" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" t="s">
+        <v>22</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="2">
+        <v>1795</v>
+      </c>
+      <c r="C95" t="s">
+        <v>28</v>
+      </c>
+      <c r="D95" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95">
+        <v>2E-3</v>
+      </c>
+      <c r="F95" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="2">
+        <v>1402810099</v>
+      </c>
+      <c r="C96" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96">
+        <v>1.3029999999999999</v>
+      </c>
+      <c r="F96" t="s">
+        <v>30</v>
+      </c>
+      <c r="G96" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="2">
+        <v>833710003</v>
+      </c>
+      <c r="C97" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97" t="s">
+        <v>22</v>
+      </c>
+      <c r="E97" s="3">
+        <v>0.59430000000000005</v>
+      </c>
+      <c r="F97" t="s">
+        <v>33</v>
+      </c>
+      <c r="G97" t="s">
+        <v>29</v>
+      </c>
+      <c r="H97" t="s">
+        <v>34</v>
+      </c>
+      <c r="I97" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="2">
+        <v>507077308</v>
+      </c>
+      <c r="C98" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98" t="s">
+        <v>22</v>
+      </c>
+      <c r="E98" s="3">
+        <v>0.36149999999999999</v>
+      </c>
+      <c r="F98" t="s">
+        <v>37</v>
+      </c>
+      <c r="G98" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" t="s">
+        <v>34</v>
+      </c>
+      <c r="I98" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="2">
+        <v>1414061707</v>
+      </c>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" t="s">
+        <v>22</v>
+      </c>
+      <c r="E99">
+        <v>1.01</v>
+      </c>
+      <c r="F99" t="s">
+        <v>40</v>
+      </c>
+      <c r="G99" t="s">
+        <v>41</v>
+      </c>
+      <c r="H99" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>22</v>
+      </c>
+      <c r="C100">
+        <v>0.59</v>
+      </c>
+      <c r="D100" t="s">
+        <v>43</v>
+      </c>
+      <c r="E100" t="s">
+        <v>29</v>
+      </c>
+      <c r="F100" t="s">
+        <v>41</v>
+      </c>
+      <c r="G100" t="s">
+        <v>44</v>
+      </c>
+      <c r="H100" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="2">
+        <v>286649193</v>
+      </c>
+      <c r="C101" t="s">
+        <v>46</v>
+      </c>
+      <c r="D101" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101">
+        <v>266.35500000000002</v>
+      </c>
+      <c r="F101" t="s">
+        <v>26</v>
+      </c>
+      <c r="G101" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="2">
+        <v>234441</v>
+      </c>
+      <c r="C102" t="s">
+        <v>48</v>
+      </c>
+      <c r="D102" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="F102" t="s">
+        <v>49</v>
+      </c>
+      <c r="G102" t="s">
+        <v>50</v>
+      </c>
+      <c r="H102" t="s">
+        <v>46</v>
+      </c>
+      <c r="I102" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gathered data on the ring buffer from cube using perf. In addition I implemented a spsc lockless ring buffer and gathered data on it from stoker, cube and my local machine both normally and with perf
</commit_message>
<xml_diff>
--- a/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
+++ b/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="115">
   <si>
     <t>Ring Buffer - Size (1000)= Doesn't matter since addition/removal is only done at the top of the queue</t>
   </si>
@@ -271,6 +271,99 @@
   </si>
   <si>
     <t>16 Core Intel CPU @ 2.27 GHz (E Cube ) Locked</t>
+  </si>
+  <si>
+    <t>Cube Locked</t>
+  </si>
+  <si>
+    <t>[84.03%]</t>
+  </si>
+  <si>
+    <t>[84.42%]</t>
+  </si>
+  <si>
+    <t>[66.92%]</t>
+  </si>
+  <si>
+    <t>[82.88%]</t>
+  </si>
+  <si>
+    <t>[82.60%]</t>
+  </si>
+  <si>
+    <t>[83.92%]</t>
+  </si>
+  <si>
+    <t>Cube TTAS</t>
+  </si>
+  <si>
+    <t>[83.81%]</t>
+  </si>
+  <si>
+    <t>[84.60%]</t>
+  </si>
+  <si>
+    <t>[64.34%]</t>
+  </si>
+  <si>
+    <t>[82.84%]</t>
+  </si>
+  <si>
+    <t>[82.93%]</t>
+  </si>
+  <si>
+    <t>[84.50%]</t>
+  </si>
+  <si>
+    <t>Cube CAS</t>
+  </si>
+  <si>
+    <t>[83.19%]</t>
+  </si>
+  <si>
+    <t>[66.87%]</t>
+  </si>
+  <si>
+    <t>[83.59%]</t>
+  </si>
+  <si>
+    <t>[83.67%]</t>
+  </si>
+  <si>
+    <t>Cube TAS</t>
+  </si>
+  <si>
+    <t>[83.50%]</t>
+  </si>
+  <si>
+    <t>[82.99%]</t>
+  </si>
+  <si>
+    <t>[83.61%]</t>
+  </si>
+  <si>
+    <t>[83.82%]</t>
+  </si>
+  <si>
+    <t>Cube Ticket</t>
+  </si>
+  <si>
+    <t>[83.39%]</t>
+  </si>
+  <si>
+    <t>[83.93%]</t>
+  </si>
+  <si>
+    <t>[66.37%]</t>
+  </si>
+  <si>
+    <t>[83.79%]</t>
+  </si>
+  <si>
+    <t>[84.11%]</t>
+  </si>
+  <si>
+    <t>[83.24%]</t>
   </si>
 </sst>
 </file>
@@ -308,11 +401,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,18 +707,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:I102"/>
+  <dimension ref="A4:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="K92" sqref="K92:S102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -660,17 +754,17 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -1336,7 +1430,7 @@
         <v>5780359</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -1365,7 +1459,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>80</v>
       </c>
@@ -1394,7 +1488,7 @@
         <v>194233</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -1423,7 +1517,7 @@
         <v>6067944</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1452,7 +1546,7 @@
         <v>262630</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1474,9 +1568,12 @@
       <c r="G40" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="2">
+      <c r="K40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
         <v>125793</v>
       </c>
       <c r="C41" t="s">
@@ -1491,8 +1588,26 @@
       <c r="F41" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>14036.038214</v>
+      </c>
+      <c r="M41" t="s">
+        <v>21</v>
+      </c>
+      <c r="N41" t="s">
+        <v>22</v>
+      </c>
+      <c r="O41">
+        <v>1.7529999999999999</v>
+      </c>
+      <c r="P41" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>895</v>
       </c>
@@ -1508,9 +1623,24 @@
       <c r="F42" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="2">
+      <c r="L42" s="1">
+        <v>77188</v>
+      </c>
+      <c r="M42" t="s">
+        <v>25</v>
+      </c>
+      <c r="N42" t="s">
+        <v>22</v>
+      </c>
+      <c r="O42">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
         <v>4880</v>
       </c>
       <c r="C43" t="s">
@@ -1525,9 +1655,24 @@
       <c r="F43" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="2">
+      <c r="L43">
+        <v>619</v>
+      </c>
+      <c r="M43" t="s">
+        <v>27</v>
+      </c>
+      <c r="N43" t="s">
+        <v>22</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
         <v>309567365952</v>
       </c>
       <c r="C44" t="s">
@@ -1545,9 +1690,24 @@
       <c r="G44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="2">
+      <c r="L44" s="1">
+        <v>6678</v>
+      </c>
+      <c r="M44" t="s">
+        <v>28</v>
+      </c>
+      <c r="N44" t="s">
+        <v>22</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
         <v>292660249898</v>
       </c>
       <c r="C45" t="s">
@@ -1556,7 +1716,7 @@
       <c r="D45" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>0.94540000000000002</v>
       </c>
       <c r="F45" t="s">
@@ -1571,9 +1731,27 @@
       <c r="I45" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="2">
+      <c r="L45" s="1">
+        <v>25111441397</v>
+      </c>
+      <c r="M45" t="s">
+        <v>29</v>
+      </c>
+      <c r="N45" t="s">
+        <v>22</v>
+      </c>
+      <c r="O45">
+        <v>1.7889999999999999</v>
+      </c>
+      <c r="P45" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
         <v>188147577898</v>
       </c>
       <c r="C46" t="s">
@@ -1582,7 +1760,7 @@
       <c r="D46" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>0.60780000000000001</v>
       </c>
       <c r="F46" t="s">
@@ -1597,9 +1775,33 @@
       <c r="I46" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="2">
+      <c r="L46" s="1">
+        <v>18202689405</v>
+      </c>
+      <c r="M46" t="s">
+        <v>32</v>
+      </c>
+      <c r="N46" t="s">
+        <v>22</v>
+      </c>
+      <c r="O46" s="2">
+        <v>0.72489999999999999</v>
+      </c>
+      <c r="P46" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>29</v>
+      </c>
+      <c r="R46" t="s">
+        <v>34</v>
+      </c>
+      <c r="S46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
         <v>30388998863</v>
       </c>
       <c r="C47" t="s">
@@ -1620,8 +1822,32 @@
       <c r="H47" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L47" s="1">
+        <v>12137295339</v>
+      </c>
+      <c r="M47" t="s">
+        <v>36</v>
+      </c>
+      <c r="N47" t="s">
+        <v>22</v>
+      </c>
+      <c r="O47" s="2">
+        <v>0.48330000000000001</v>
+      </c>
+      <c r="P47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>29</v>
+      </c>
+      <c r="R47" t="s">
+        <v>34</v>
+      </c>
+      <c r="S47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>22</v>
       </c>
@@ -1643,9 +1869,30 @@
       <c r="H48" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="2">
+      <c r="L48" s="1">
+        <v>15376853332</v>
+      </c>
+      <c r="M48" t="s">
+        <v>39</v>
+      </c>
+      <c r="N48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O48">
+        <v>0.61</v>
+      </c>
+      <c r="P48" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>41</v>
+      </c>
+      <c r="R48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
         <v>10528527003</v>
       </c>
       <c r="C49" t="s">
@@ -1663,9 +1910,30 @@
       <c r="G49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="2">
+      <c r="L49" t="s">
+        <v>22</v>
+      </c>
+      <c r="M49">
+        <v>1.18</v>
+      </c>
+      <c r="N49" t="s">
+        <v>43</v>
+      </c>
+      <c r="O49" t="s">
+        <v>29</v>
+      </c>
+      <c r="P49" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>44</v>
+      </c>
+      <c r="R49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
         <v>9315830</v>
       </c>
       <c r="C50" t="s">
@@ -1674,7 +1942,7 @@
       <c r="D50" t="s">
         <v>22</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>8.9999999999999998E-4</v>
       </c>
       <c r="F50" t="s">
@@ -1689,13 +1957,60 @@
       <c r="I50" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L50" s="1">
+        <v>3795939390</v>
+      </c>
+      <c r="M50" t="s">
+        <v>46</v>
+      </c>
+      <c r="N50" t="s">
+        <v>22</v>
+      </c>
+      <c r="O50">
+        <v>270.44200000000001</v>
+      </c>
+      <c r="P50" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L51" s="1">
+        <v>4077057</v>
+      </c>
+      <c r="M51" t="s">
+        <v>48</v>
+      </c>
+      <c r="N51" t="s">
+        <v>22</v>
+      </c>
+      <c r="O51" s="2">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="P51" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>50</v>
+      </c>
+      <c r="R51" t="s">
+        <v>46</v>
+      </c>
+      <c r="S51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>10695.285760999999</v>
       </c>
@@ -1715,8 +2030,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
         <v>309495</v>
       </c>
       <c r="C54" t="s">
@@ -1731,9 +2046,27 @@
       <c r="F54" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="2">
+      <c r="L54">
+        <v>9256.1163730000007</v>
+      </c>
+      <c r="M54" t="s">
+        <v>21</v>
+      </c>
+      <c r="N54" t="s">
+        <v>22</v>
+      </c>
+      <c r="O54">
+        <v>1.1559999999999999</v>
+      </c>
+      <c r="P54" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
         <v>5967</v>
       </c>
       <c r="C55" t="s">
@@ -1748,9 +2081,24 @@
       <c r="F55" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="2">
+      <c r="L55" s="1">
+        <v>279820</v>
+      </c>
+      <c r="M55" t="s">
+        <v>25</v>
+      </c>
+      <c r="N55" t="s">
+        <v>22</v>
+      </c>
+      <c r="O55">
+        <v>0.03</v>
+      </c>
+      <c r="P55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
         <v>6308</v>
       </c>
       <c r="C56" t="s">
@@ -1765,9 +2113,24 @@
       <c r="F56" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="2">
+      <c r="L56" s="1">
+        <v>9293</v>
+      </c>
+      <c r="M56" t="s">
+        <v>27</v>
+      </c>
+      <c r="N56" t="s">
+        <v>22</v>
+      </c>
+      <c r="O56">
+        <v>1E-3</v>
+      </c>
+      <c r="P56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
         <v>11270458403</v>
       </c>
       <c r="C57" t="s">
@@ -1785,9 +2148,24 @@
       <c r="G57" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="2">
+      <c r="L57" s="1">
+        <v>4912</v>
+      </c>
+      <c r="M57" t="s">
+        <v>28</v>
+      </c>
+      <c r="N57" t="s">
+        <v>22</v>
+      </c>
+      <c r="O57">
+        <v>1E-3</v>
+      </c>
+      <c r="P57" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
         <v>6848111760</v>
       </c>
       <c r="C58" t="s">
@@ -1796,7 +2174,7 @@
       <c r="D58" t="s">
         <v>22</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="2">
         <v>0.60760000000000003</v>
       </c>
       <c r="F58" t="s">
@@ -1811,9 +2189,27 @@
       <c r="I58" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="2">
+      <c r="L58" s="1">
+        <v>15693907274</v>
+      </c>
+      <c r="M58" t="s">
+        <v>29</v>
+      </c>
+      <c r="N58" t="s">
+        <v>22</v>
+      </c>
+      <c r="O58">
+        <v>1.696</v>
+      </c>
+      <c r="P58" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
         <v>4364938024</v>
       </c>
       <c r="C59" t="s">
@@ -1822,7 +2218,7 @@
       <c r="D59" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="2">
         <v>0.38729999999999998</v>
       </c>
       <c r="F59" t="s">
@@ -1837,9 +2233,33 @@
       <c r="I59" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="2">
+      <c r="L59" s="1">
+        <v>9411716033</v>
+      </c>
+      <c r="M59" t="s">
+        <v>32</v>
+      </c>
+      <c r="N59" t="s">
+        <v>22</v>
+      </c>
+      <c r="O59" s="2">
+        <v>0.59970000000000001</v>
+      </c>
+      <c r="P59" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>29</v>
+      </c>
+      <c r="R59" t="s">
+        <v>34</v>
+      </c>
+      <c r="S59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
         <v>9661845211</v>
       </c>
       <c r="C60" t="s">
@@ -1860,8 +2280,32 @@
       <c r="H60" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L60" s="1">
+        <v>6339497977</v>
+      </c>
+      <c r="M60" t="s">
+        <v>36</v>
+      </c>
+      <c r="N60" t="s">
+        <v>22</v>
+      </c>
+      <c r="O60" s="2">
+        <v>0.40389999999999998</v>
+      </c>
+      <c r="P60" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>29</v>
+      </c>
+      <c r="R60" t="s">
+        <v>34</v>
+      </c>
+      <c r="S60" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>22</v>
       </c>
@@ -1883,9 +2327,30 @@
       <c r="H61" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="2">
+      <c r="L61" s="1">
+        <v>14512658926</v>
+      </c>
+      <c r="M61" t="s">
+        <v>39</v>
+      </c>
+      <c r="N61" t="s">
+        <v>22</v>
+      </c>
+      <c r="O61">
+        <v>0.92</v>
+      </c>
+      <c r="P61" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>41</v>
+      </c>
+      <c r="R61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
         <v>1920524089</v>
       </c>
       <c r="C62" t="s">
@@ -1903,9 +2368,30 @@
       <c r="G62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="2">
+      <c r="L62" t="s">
+        <v>22</v>
+      </c>
+      <c r="M62">
+        <v>0.65</v>
+      </c>
+      <c r="N62" t="s">
+        <v>43</v>
+      </c>
+      <c r="O62" t="s">
+        <v>29</v>
+      </c>
+      <c r="P62" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>44</v>
+      </c>
+      <c r="R62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B63" s="1">
         <v>7340566</v>
       </c>
       <c r="C63" t="s">
@@ -1914,7 +2400,7 @@
       <c r="D63" t="s">
         <v>22</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="2">
         <v>3.8E-3</v>
       </c>
       <c r="F63" t="s">
@@ -1929,13 +2415,60 @@
       <c r="I63" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L63" s="1">
+        <v>2867603960</v>
+      </c>
+      <c r="M63" t="s">
+        <v>46</v>
+      </c>
+      <c r="N63" t="s">
+        <v>22</v>
+      </c>
+      <c r="O63">
+        <v>309.80599999999998</v>
+      </c>
+      <c r="P63" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L64" s="1">
+        <v>7920589</v>
+      </c>
+      <c r="M64" t="s">
+        <v>48</v>
+      </c>
+      <c r="N64" t="s">
+        <v>22</v>
+      </c>
+      <c r="O64" s="2">
+        <v>2.8E-3</v>
+      </c>
+      <c r="P64" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>50</v>
+      </c>
+      <c r="R64" t="s">
+        <v>46</v>
+      </c>
+      <c r="S64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K65" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>8045.4323169999998</v>
       </c>
@@ -1954,9 +2487,27 @@
       <c r="G66" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="2">
+      <c r="L66">
+        <v>8019.0536229999998</v>
+      </c>
+      <c r="M66" t="s">
+        <v>21</v>
+      </c>
+      <c r="N66" t="s">
+        <v>22</v>
+      </c>
+      <c r="O66">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="P66" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
         <v>526</v>
       </c>
       <c r="C67" t="s">
@@ -1971,9 +2522,24 @@
       <c r="F67" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B68" s="2">
+      <c r="L67">
+        <v>594</v>
+      </c>
+      <c r="M67" t="s">
+        <v>25</v>
+      </c>
+      <c r="N67" t="s">
+        <v>22</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
         <v>273</v>
       </c>
       <c r="C68" t="s">
@@ -1988,9 +2554,24 @@
       <c r="F68" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B69" s="2">
+      <c r="L68">
+        <v>343</v>
+      </c>
+      <c r="M68" t="s">
+        <v>27</v>
+      </c>
+      <c r="N68" t="s">
+        <v>22</v>
+      </c>
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="P68" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
         <v>3759</v>
       </c>
       <c r="C69" t="s">
@@ -2005,9 +2586,24 @@
       <c r="F69" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B70" s="2">
+      <c r="L69" s="1">
+        <v>4726</v>
+      </c>
+      <c r="M69" t="s">
+        <v>28</v>
+      </c>
+      <c r="N69" t="s">
+        <v>22</v>
+      </c>
+      <c r="O69">
+        <v>1E-3</v>
+      </c>
+      <c r="P69" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
         <v>12801950363</v>
       </c>
       <c r="C70" t="s">
@@ -2025,9 +2621,27 @@
       <c r="G70" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="2">
+      <c r="L70" s="1">
+        <v>14836125712</v>
+      </c>
+      <c r="M70" t="s">
+        <v>29</v>
+      </c>
+      <c r="N70" t="s">
+        <v>22</v>
+      </c>
+      <c r="O70">
+        <v>1.85</v>
+      </c>
+      <c r="P70" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
         <v>7550260810</v>
       </c>
       <c r="C71" t="s">
@@ -2036,7 +2650,7 @@
       <c r="D71" t="s">
         <v>22</v>
       </c>
-      <c r="E71" s="3">
+      <c r="E71" s="2">
         <v>0.58979999999999999</v>
       </c>
       <c r="F71" t="s">
@@ -2051,9 +2665,33 @@
       <c r="I71" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="2">
+      <c r="L71" s="1">
+        <v>8686638292</v>
+      </c>
+      <c r="M71" t="s">
+        <v>32</v>
+      </c>
+      <c r="N71" t="s">
+        <v>22</v>
+      </c>
+      <c r="O71" s="2">
+        <v>0.58550000000000002</v>
+      </c>
+      <c r="P71" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>29</v>
+      </c>
+      <c r="R71" t="s">
+        <v>34</v>
+      </c>
+      <c r="S71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
         <v>4569939952</v>
       </c>
       <c r="C72" t="s">
@@ -2062,7 +2700,7 @@
       <c r="D72" t="s">
         <v>22</v>
       </c>
-      <c r="E72" s="3">
+      <c r="E72" s="2">
         <v>0.35699999999999998</v>
       </c>
       <c r="F72" t="s">
@@ -2077,9 +2715,33 @@
       <c r="I72" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="2">
+      <c r="L72" s="1">
+        <v>5622799957</v>
+      </c>
+      <c r="M72" t="s">
+        <v>36</v>
+      </c>
+      <c r="N72" t="s">
+        <v>22</v>
+      </c>
+      <c r="O72" s="2">
+        <v>0.379</v>
+      </c>
+      <c r="P72" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>29</v>
+      </c>
+      <c r="R72" t="s">
+        <v>34</v>
+      </c>
+      <c r="S72" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B73" s="1">
         <v>13025703849</v>
       </c>
       <c r="C73" t="s">
@@ -2100,8 +2762,29 @@
       <c r="H73" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L73" s="1">
+        <v>14767034841</v>
+      </c>
+      <c r="M73" t="s">
+        <v>39</v>
+      </c>
+      <c r="N73" t="s">
+        <v>22</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>41</v>
+      </c>
+      <c r="R73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>22</v>
       </c>
@@ -2123,9 +2806,30 @@
       <c r="H74" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B75" s="2">
+      <c r="L74" t="s">
+        <v>22</v>
+      </c>
+      <c r="M74">
+        <v>0.59</v>
+      </c>
+      <c r="N74" t="s">
+        <v>43</v>
+      </c>
+      <c r="O74" t="s">
+        <v>29</v>
+      </c>
+      <c r="P74" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>44</v>
+      </c>
+      <c r="R74" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B75" s="1">
         <v>2506811383</v>
       </c>
       <c r="C75" t="s">
@@ -2143,9 +2847,27 @@
       <c r="G75" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="2">
+      <c r="L75" s="1">
+        <v>2788052548</v>
+      </c>
+      <c r="M75" t="s">
+        <v>46</v>
+      </c>
+      <c r="N75" t="s">
+        <v>22</v>
+      </c>
+      <c r="O75">
+        <v>347.67899999999997</v>
+      </c>
+      <c r="P75" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B76" s="1">
         <v>236508</v>
       </c>
       <c r="C76" t="s">
@@ -2154,7 +2876,7 @@
       <c r="D76" t="s">
         <v>22</v>
       </c>
-      <c r="E76" s="3">
+      <c r="E76" s="2">
         <v>1E-4</v>
       </c>
       <c r="F76" t="s">
@@ -2169,13 +2891,40 @@
       <c r="I76" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L76" s="1">
+        <v>225594</v>
+      </c>
+      <c r="M76" t="s">
+        <v>48</v>
+      </c>
+      <c r="N76" t="s">
+        <v>22</v>
+      </c>
+      <c r="O76" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="P76" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>50</v>
+      </c>
+      <c r="R76" t="s">
+        <v>46</v>
+      </c>
+      <c r="S76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K78" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>188185.89483400001</v>
       </c>
@@ -2194,9 +2943,27 @@
       <c r="G79" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B80" s="2">
+      <c r="L79">
+        <v>55673.967834000003</v>
+      </c>
+      <c r="M79" t="s">
+        <v>21</v>
+      </c>
+      <c r="N79" t="s">
+        <v>22</v>
+      </c>
+      <c r="O79">
+        <v>6.9530000000000003</v>
+      </c>
+      <c r="P79" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B80" s="1">
         <v>4235</v>
       </c>
       <c r="C80" t="s">
@@ -2211,9 +2978,24 @@
       <c r="F80" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="2">
+      <c r="L80" s="1">
+        <v>3627</v>
+      </c>
+      <c r="M80" t="s">
+        <v>25</v>
+      </c>
+      <c r="N80" t="s">
+        <v>22</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="P80" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B81" s="1">
         <v>329</v>
       </c>
       <c r="C81" t="s">
@@ -2228,9 +3010,24 @@
       <c r="F81" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="2">
+      <c r="L81">
+        <v>445</v>
+      </c>
+      <c r="M81" t="s">
+        <v>27</v>
+      </c>
+      <c r="N81" t="s">
+        <v>22</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
+      </c>
+      <c r="P81" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B82" s="1">
         <v>2388</v>
       </c>
       <c r="C82" t="s">
@@ -2245,9 +3042,24 @@
       <c r="F82" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="2">
+      <c r="L82" s="1">
+        <v>7426</v>
+      </c>
+      <c r="M82" t="s">
+        <v>28</v>
+      </c>
+      <c r="N82" t="s">
+        <v>22</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+      <c r="P82" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B83" s="1">
         <v>391423099860</v>
       </c>
       <c r="C83" t="s">
@@ -2265,9 +3077,27 @@
       <c r="G83" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B84" s="2">
+      <c r="L83" s="1">
+        <v>126525316304</v>
+      </c>
+      <c r="M83" t="s">
+        <v>29</v>
+      </c>
+      <c r="N83" t="s">
+        <v>22</v>
+      </c>
+      <c r="O83">
+        <v>2.2730000000000001</v>
+      </c>
+      <c r="P83" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B84" s="1">
         <v>387870592065</v>
       </c>
       <c r="C84" t="s">
@@ -2276,7 +3106,7 @@
       <c r="D84" t="s">
         <v>22</v>
       </c>
-      <c r="E84" s="3">
+      <c r="E84" s="2">
         <v>0.9909</v>
       </c>
       <c r="F84" t="s">
@@ -2291,9 +3121,33 @@
       <c r="I84" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="2">
+      <c r="L84" s="1">
+        <v>122810006653</v>
+      </c>
+      <c r="M84" t="s">
+        <v>32</v>
+      </c>
+      <c r="N84" t="s">
+        <v>22</v>
+      </c>
+      <c r="O84" s="2">
+        <v>0.97060000000000002</v>
+      </c>
+      <c r="P84" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>29</v>
+      </c>
+      <c r="R84" t="s">
+        <v>34</v>
+      </c>
+      <c r="S84" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B85" s="1">
         <v>327940949960</v>
       </c>
       <c r="C85" t="s">
@@ -2302,7 +3156,7 @@
       <c r="D85" t="s">
         <v>22</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E85" s="2">
         <v>0.83779999999999999</v>
       </c>
       <c r="F85" t="s">
@@ -2317,9 +3171,33 @@
       <c r="I85" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="2">
+      <c r="L85" s="1">
+        <v>107562363039</v>
+      </c>
+      <c r="M85" t="s">
+        <v>36</v>
+      </c>
+      <c r="N85" t="s">
+        <v>22</v>
+      </c>
+      <c r="O85" s="2">
+        <v>0.85009999999999997</v>
+      </c>
+      <c r="P85" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>29</v>
+      </c>
+      <c r="R85" t="s">
+        <v>34</v>
+      </c>
+      <c r="S85" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B86" s="1">
         <v>9389575924</v>
       </c>
       <c r="C86" t="s">
@@ -2340,8 +3218,29 @@
       <c r="H86" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L86" s="1">
+        <v>8354453323</v>
+      </c>
+      <c r="M86" t="s">
+        <v>39</v>
+      </c>
+      <c r="N86" t="s">
+        <v>22</v>
+      </c>
+      <c r="O86">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P86" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>41</v>
+      </c>
+      <c r="R86" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>22</v>
       </c>
@@ -2363,9 +3262,30 @@
       <c r="H87" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B88" s="2">
+      <c r="L87" t="s">
+        <v>22</v>
+      </c>
+      <c r="M87">
+        <v>14.7</v>
+      </c>
+      <c r="N87" t="s">
+        <v>43</v>
+      </c>
+      <c r="O87" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>44</v>
+      </c>
+      <c r="R87" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B88" s="1">
         <v>1651093111</v>
       </c>
       <c r="C88" t="s">
@@ -2383,9 +3303,27 @@
       <c r="G88" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="2">
+      <c r="L88" s="1">
+        <v>1446943226</v>
+      </c>
+      <c r="M88" t="s">
+        <v>46</v>
+      </c>
+      <c r="N88" t="s">
+        <v>22</v>
+      </c>
+      <c r="O88">
+        <v>25.99</v>
+      </c>
+      <c r="P88" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B89" s="1">
         <v>2658981</v>
       </c>
       <c r="C89" t="s">
@@ -2394,7 +3332,7 @@
       <c r="D89" t="s">
         <v>22</v>
       </c>
-      <c r="E89" s="3">
+      <c r="E89" s="2">
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="F89" t="s">
@@ -2409,13 +3347,40 @@
       <c r="I89" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L89" s="1">
+        <v>9008285</v>
+      </c>
+      <c r="M89" t="s">
+        <v>48</v>
+      </c>
+      <c r="N89" t="s">
+        <v>22</v>
+      </c>
+      <c r="O89" s="2">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="P89" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>50</v>
+      </c>
+      <c r="R89" t="s">
+        <v>46</v>
+      </c>
+      <c r="S89" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K91" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>1076.193186</v>
       </c>
@@ -2434,8 +3399,26 @@
       <c r="G92" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L92">
+        <v>1046.769121</v>
+      </c>
+      <c r="M92" t="s">
+        <v>21</v>
+      </c>
+      <c r="N92" t="s">
+        <v>22</v>
+      </c>
+      <c r="O92">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P92" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>503</v>
       </c>
@@ -2451,8 +3434,23 @@
       <c r="F93" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L93">
+        <v>597</v>
+      </c>
+      <c r="M93" t="s">
+        <v>25</v>
+      </c>
+      <c r="N93" t="s">
+        <v>22</v>
+      </c>
+      <c r="O93">
+        <v>1E-3</v>
+      </c>
+      <c r="P93" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>257</v>
       </c>
@@ -2468,9 +3466,24 @@
       <c r="F94" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="2">
+      <c r="L94">
+        <v>262</v>
+      </c>
+      <c r="M94" t="s">
+        <v>27</v>
+      </c>
+      <c r="N94" t="s">
+        <v>22</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="P94" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B95" s="1">
         <v>1795</v>
       </c>
       <c r="C95" t="s">
@@ -2485,9 +3498,24 @@
       <c r="F95" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B96" s="2">
+      <c r="L95" s="1">
+        <v>1794</v>
+      </c>
+      <c r="M95" t="s">
+        <v>28</v>
+      </c>
+      <c r="N95" t="s">
+        <v>22</v>
+      </c>
+      <c r="O95">
+        <v>2E-3</v>
+      </c>
+      <c r="P95" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B96" s="1">
         <v>1402810099</v>
       </c>
       <c r="C96" t="s">
@@ -2505,9 +3533,27 @@
       <c r="G96" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B97" s="2">
+      <c r="L96" s="1">
+        <v>1668027061</v>
+      </c>
+      <c r="M96" t="s">
+        <v>29</v>
+      </c>
+      <c r="N96" t="s">
+        <v>22</v>
+      </c>
+      <c r="O96">
+        <v>1.5940000000000001</v>
+      </c>
+      <c r="P96" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B97" s="1">
         <v>833710003</v>
       </c>
       <c r="C97" t="s">
@@ -2516,7 +3562,7 @@
       <c r="D97" t="s">
         <v>22</v>
       </c>
-      <c r="E97" s="3">
+      <c r="E97" s="2">
         <v>0.59430000000000005</v>
       </c>
       <c r="F97" t="s">
@@ -2531,9 +3577,33 @@
       <c r="I97" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B98" s="2">
+      <c r="L97" s="1">
+        <v>999157649</v>
+      </c>
+      <c r="M97" t="s">
+        <v>32</v>
+      </c>
+      <c r="N97" t="s">
+        <v>22</v>
+      </c>
+      <c r="O97" s="2">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="P97" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>29</v>
+      </c>
+      <c r="R97" t="s">
+        <v>34</v>
+      </c>
+      <c r="S97" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="98" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B98" s="1">
         <v>507077308</v>
       </c>
       <c r="C98" t="s">
@@ -2542,7 +3612,7 @@
       <c r="D98" t="s">
         <v>22</v>
       </c>
-      <c r="E98" s="3">
+      <c r="E98" s="2">
         <v>0.36149999999999999</v>
       </c>
       <c r="F98" t="s">
@@ -2557,9 +3627,33 @@
       <c r="I98" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="2">
+      <c r="L98" s="1">
+        <v>656082373</v>
+      </c>
+      <c r="M98" t="s">
+        <v>36</v>
+      </c>
+      <c r="N98" t="s">
+        <v>22</v>
+      </c>
+      <c r="O98" s="2">
+        <v>0.39329999999999998</v>
+      </c>
+      <c r="P98" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>29</v>
+      </c>
+      <c r="R98" t="s">
+        <v>34</v>
+      </c>
+      <c r="S98" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B99" s="1">
         <v>1414061707</v>
       </c>
       <c r="C99" t="s">
@@ -2580,8 +3674,29 @@
       <c r="H99" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L99" s="1">
+        <v>1640791508</v>
+      </c>
+      <c r="M99" t="s">
+        <v>39</v>
+      </c>
+      <c r="N99" t="s">
+        <v>22</v>
+      </c>
+      <c r="O99">
+        <v>0.98</v>
+      </c>
+      <c r="P99" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>41</v>
+      </c>
+      <c r="R99" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>22</v>
       </c>
@@ -2603,9 +3718,30 @@
       <c r="H100" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B101" s="2">
+      <c r="L100" t="s">
+        <v>22</v>
+      </c>
+      <c r="M100">
+        <v>0.61</v>
+      </c>
+      <c r="N100" t="s">
+        <v>43</v>
+      </c>
+      <c r="O100" t="s">
+        <v>29</v>
+      </c>
+      <c r="P100" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>44</v>
+      </c>
+      <c r="R100" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B101" s="1">
         <v>286649193</v>
       </c>
       <c r="C101" t="s">
@@ -2623,9 +3759,27 @@
       <c r="G101" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B102" s="2">
+      <c r="L101" s="1">
+        <v>331694921</v>
+      </c>
+      <c r="M101" t="s">
+        <v>46</v>
+      </c>
+      <c r="N101" t="s">
+        <v>22</v>
+      </c>
+      <c r="O101">
+        <v>316.875</v>
+      </c>
+      <c r="P101" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="102" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B102" s="1">
         <v>234441</v>
       </c>
       <c r="C102" t="s">
@@ -2634,7 +3788,7 @@
       <c r="D102" t="s">
         <v>22</v>
       </c>
-      <c r="E102" s="3">
+      <c r="E102" s="2">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="F102" t="s">
@@ -2648,6 +3802,30 @@
       </c>
       <c r="I102" t="s">
         <v>74</v>
+      </c>
+      <c r="L102" s="1">
+        <v>270404</v>
+      </c>
+      <c r="M102" t="s">
+        <v>48</v>
+      </c>
+      <c r="N102" t="s">
+        <v>22</v>
+      </c>
+      <c r="O102" s="2">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="P102" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>50</v>
+      </c>
+      <c r="R102" t="s">
+        <v>46</v>
+      </c>
+      <c r="S102" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented locked MPMC, found in buffer_mpmc.cpp and gathered data from both locked and lockess variations, storing the data in MPMC_BUFFER_TEST_DATA
</commit_message>
<xml_diff>
--- a/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
+++ b/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
@@ -532,7 +532,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1535,11 +1534,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99316096"/>
-        <c:axId val="99318016"/>
+        <c:axId val="69382528"/>
+        <c:axId val="69384448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99316096"/>
+        <c:axId val="69382528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,14 +1560,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99318016"/>
+        <c:crossAx val="69384448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1576,7 +1574,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99318016"/>
+        <c:axId val="69384448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1599,21 +1597,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99316096"/>
+        <c:crossAx val="69382528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1930,11 +1926,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101615872"/>
-        <c:axId val="101622144"/>
+        <c:axId val="72292608"/>
+        <c:axId val="72323456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101615872"/>
+        <c:axId val="72292608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1963,7 +1959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101622144"/>
+        <c:crossAx val="72323456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1971,7 +1967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101622144"/>
+        <c:axId val="72323456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2001,7 +1997,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101615872"/>
+        <c:crossAx val="72292608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2564,11 +2560,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106454016"/>
-        <c:axId val="106460288"/>
+        <c:axId val="72360704"/>
+        <c:axId val="72362624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106454016"/>
+        <c:axId val="72360704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2597,7 +2593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106460288"/>
+        <c:crossAx val="72362624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2605,7 +2601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106460288"/>
+        <c:axId val="72362624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2635,7 +2631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106454016"/>
+        <c:crossAx val="72360704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3198,11 +3194,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106487808"/>
-        <c:axId val="106489728"/>
+        <c:axId val="78056448"/>
+        <c:axId val="78058624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106487808"/>
+        <c:axId val="78056448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3231,7 +3227,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106489728"/>
+        <c:crossAx val="78058624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3239,7 +3235,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106489728"/>
+        <c:axId val="78058624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3269,7 +3265,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106487808"/>
+        <c:crossAx val="78056448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3839,11 +3835,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106541824"/>
-        <c:axId val="106543744"/>
+        <c:axId val="78095872"/>
+        <c:axId val="78097792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106541824"/>
+        <c:axId val="78095872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3872,7 +3868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106543744"/>
+        <c:crossAx val="78097792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3880,7 +3876,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106543744"/>
+        <c:axId val="78097792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3910,7 +3906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106541824"/>
+        <c:crossAx val="78095872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4724,11 +4720,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="58357632"/>
-        <c:axId val="58372480"/>
+        <c:axId val="78240000"/>
+        <c:axId val="78246272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58357632"/>
+        <c:axId val="78240000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4757,7 +4753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58372480"/>
+        <c:crossAx val="78246272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4765,7 +4761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58372480"/>
+        <c:axId val="78246272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4795,7 +4791,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58357632"/>
+        <c:crossAx val="78240000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5363,11 +5359,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45910656"/>
-        <c:axId val="57525376"/>
+        <c:axId val="78156544"/>
+        <c:axId val="78158464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45910656"/>
+        <c:axId val="78156544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5396,7 +5392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57525376"/>
+        <c:crossAx val="78158464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5404,7 +5400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57525376"/>
+        <c:axId val="78158464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5434,7 +5430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45910656"/>
+        <c:crossAx val="78156544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6501,11 +6497,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100875648"/>
-        <c:axId val="100894208"/>
+        <c:axId val="69328256"/>
+        <c:axId val="69334528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100875648"/>
+        <c:axId val="69328256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6527,14 +6523,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100894208"/>
+        <c:crossAx val="69334528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6542,7 +6537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100894208"/>
+        <c:axId val="69334528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6565,21 +6560,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100875648"/>
+        <c:crossAx val="69328256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6629,7 +6622,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7632,11 +7624,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101452800"/>
-        <c:axId val="101463168"/>
+        <c:axId val="72133248"/>
+        <c:axId val="72147712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101452800"/>
+        <c:axId val="72133248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7658,14 +7650,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101463168"/>
+        <c:crossAx val="72147712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7673,7 +7664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101463168"/>
+        <c:axId val="72147712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7696,21 +7687,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101452800"/>
+        <c:crossAx val="72133248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8020,11 +8009,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101489280"/>
-        <c:axId val="101491456"/>
+        <c:axId val="71989888"/>
+        <c:axId val="71992064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101489280"/>
+        <c:axId val="71989888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8053,7 +8042,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101491456"/>
+        <c:crossAx val="71992064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8061,7 +8050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101491456"/>
+        <c:axId val="71992064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8091,7 +8080,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101489280"/>
+        <c:crossAx val="71989888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8408,11 +8397,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101329536"/>
-        <c:axId val="101335808"/>
+        <c:axId val="72041216"/>
+        <c:axId val="72043136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101329536"/>
+        <c:axId val="72041216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8441,7 +8430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101335808"/>
+        <c:crossAx val="72043136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8449,7 +8438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101335808"/>
+        <c:axId val="72043136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8479,7 +8468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101329536"/>
+        <c:crossAx val="72041216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8796,11 +8785,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101382784"/>
-        <c:axId val="101389056"/>
+        <c:axId val="72078080"/>
+        <c:axId val="72080000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101382784"/>
+        <c:axId val="72078080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8829,7 +8818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101389056"/>
+        <c:crossAx val="72080000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8837,7 +8826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101389056"/>
+        <c:axId val="72080000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8867,7 +8856,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101382784"/>
+        <c:crossAx val="72078080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9191,11 +9180,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101411456"/>
-        <c:axId val="101434112"/>
+        <c:axId val="72434432"/>
+        <c:axId val="72436352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101411456"/>
+        <c:axId val="72434432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9224,7 +9213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101434112"/>
+        <c:crossAx val="72436352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9232,7 +9221,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101434112"/>
+        <c:axId val="72436352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9262,7 +9251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101411456"/>
+        <c:crossAx val="72434432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9583,11 +9572,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101661312"/>
-        <c:axId val="101667584"/>
+        <c:axId val="72475392"/>
+        <c:axId val="72477312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101661312"/>
+        <c:axId val="72475392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9615,7 +9604,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101667584"/>
+        <c:crossAx val="72477312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9623,7 +9612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101667584"/>
+        <c:axId val="72477312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9652,7 +9641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101661312"/>
+        <c:crossAx val="72475392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9968,11 +9957,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101693696"/>
-        <c:axId val="101699968"/>
+        <c:axId val="72273920"/>
+        <c:axId val="72275840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101693696"/>
+        <c:axId val="72273920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10001,7 +9990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101699968"/>
+        <c:crossAx val="72275840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10009,7 +9998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101699968"/>
+        <c:axId val="72275840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10039,7 +10028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101693696"/>
+        <c:crossAx val="72273920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10381,16 +10370,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10417,10 +10406,10 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10444,15 +10433,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10475,16 +10464,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10507,16 +10496,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10829,7 +10818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:S123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J23" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated previous data with 128 key ranges and perf data
</commit_message>
<xml_diff>
--- a/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
+++ b/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="158">
   <si>
     <t>Ring Buffer - Size (1000)= Doesn't matter since addition/removal is only done at the top of the queue</t>
   </si>
@@ -428,6 +428,72 @@
   <si>
     <t>16 Core Intel CPU @ 2.27 GHz (E ) TICKET_RELAX</t>
   </si>
+  <si>
+    <t>NOTE 128 DATA FURTHER DOWN</t>
+  </si>
+  <si>
+    <t>cache-references</t>
+  </si>
+  <si>
+    <t>cache-misses</t>
+  </si>
+  <si>
+    <t>bus-cycles</t>
+  </si>
+  <si>
+    <t>faults</t>
+  </si>
+  <si>
+    <t>cpu-clock</t>
+  </si>
+  <si>
+    <t>Stoker TTAS</t>
+  </si>
+  <si>
+    <t>Stoker TTASNP</t>
+  </si>
+  <si>
+    <t>Cube TTASNP</t>
+  </si>
+  <si>
+    <t>Stoker CASLOCK</t>
+  </si>
+  <si>
+    <t>Cube CASLOCK</t>
+  </si>
+  <si>
+    <t>Stoker TAS</t>
+  </si>
+  <si>
+    <t>Stoker TASWP</t>
+  </si>
+  <si>
+    <t>Cube TASWP</t>
+  </si>
+  <si>
+    <t>Stoker Ticket</t>
+  </si>
+  <si>
+    <t>Stoker TTAS_RELAX</t>
+  </si>
+  <si>
+    <t>Cube TTAS_RELAX</t>
+  </si>
+  <si>
+    <t>Stoker TICKET_RELAX</t>
+  </si>
+  <si>
+    <t>Cube TICKET_RELAX</t>
+  </si>
+  <si>
+    <t>Stoker TAS_RELAX</t>
+  </si>
+  <si>
+    <t>Cube TAS_RELAX</t>
+  </si>
+  <si>
+    <t>128 DATA &amp; PERF BELOW CAS Blanks were due to seg faults</t>
+  </si>
 </sst>
 </file>
 
@@ -452,12 +518,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -473,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -482,6 +554,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -532,6 +605,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1534,11 +1608,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69382528"/>
-        <c:axId val="69384448"/>
+        <c:axId val="97112448"/>
+        <c:axId val="97114368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69382528"/>
+        <c:axId val="97112448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,13 +1634,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69384448"/>
+        <c:crossAx val="97114368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1574,7 +1649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69384448"/>
+        <c:axId val="97114368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,19 +1672,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69382528"/>
+        <c:crossAx val="97112448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1926,11 +2003,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72292608"/>
-        <c:axId val="72323456"/>
+        <c:axId val="100014720"/>
+        <c:axId val="100041472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72292608"/>
+        <c:axId val="100014720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,7 +2036,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72323456"/>
+        <c:crossAx val="100041472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1967,7 +2044,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72323456"/>
+        <c:axId val="100041472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +2074,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72292608"/>
+        <c:crossAx val="100014720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2560,11 +2637,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72360704"/>
-        <c:axId val="72362624"/>
+        <c:axId val="100684544"/>
+        <c:axId val="100686464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72360704"/>
+        <c:axId val="100684544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2593,7 +2670,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72362624"/>
+        <c:crossAx val="100686464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2601,7 +2678,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72362624"/>
+        <c:axId val="100686464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2631,7 +2708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72360704"/>
+        <c:crossAx val="100684544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3194,11 +3271,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="78056448"/>
-        <c:axId val="78058624"/>
+        <c:axId val="100731904"/>
+        <c:axId val="100734080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78056448"/>
+        <c:axId val="100731904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3227,7 +3304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78058624"/>
+        <c:crossAx val="100734080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3235,7 +3312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78058624"/>
+        <c:axId val="100734080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,7 +3342,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78056448"/>
+        <c:crossAx val="100731904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3835,11 +3912,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="78095872"/>
-        <c:axId val="78097792"/>
+        <c:axId val="100783616"/>
+        <c:axId val="100785536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78095872"/>
+        <c:axId val="100783616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3868,7 +3945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78097792"/>
+        <c:crossAx val="100785536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3876,7 +3953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78097792"/>
+        <c:axId val="100785536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3906,7 +3983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78095872"/>
+        <c:crossAx val="100783616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4720,11 +4797,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="78240000"/>
-        <c:axId val="78246272"/>
+        <c:axId val="106551552"/>
+        <c:axId val="106557824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78240000"/>
+        <c:axId val="106551552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4753,7 +4830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78246272"/>
+        <c:crossAx val="106557824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4761,7 +4838,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78246272"/>
+        <c:axId val="106557824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4791,7 +4868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78240000"/>
+        <c:crossAx val="106551552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5359,11 +5436,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="78156544"/>
-        <c:axId val="78158464"/>
+        <c:axId val="106599168"/>
+        <c:axId val="106601088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78156544"/>
+        <c:axId val="106599168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5392,7 +5469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78158464"/>
+        <c:crossAx val="106601088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5400,7 +5477,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78158464"/>
+        <c:axId val="106601088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5430,7 +5507,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78156544"/>
+        <c:crossAx val="106599168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6497,11 +6574,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69328256"/>
-        <c:axId val="69334528"/>
+        <c:axId val="97189248"/>
+        <c:axId val="98702848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69328256"/>
+        <c:axId val="97189248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6523,13 +6600,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69334528"/>
+        <c:crossAx val="98702848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6537,7 +6615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69334528"/>
+        <c:axId val="98702848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6560,19 +6638,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69328256"/>
+        <c:crossAx val="97189248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7624,11 +7704,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72133248"/>
-        <c:axId val="72147712"/>
+        <c:axId val="98749056"/>
+        <c:axId val="98759424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72133248"/>
+        <c:axId val="98749056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7656,7 +7736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72147712"/>
+        <c:crossAx val="98759424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7664,7 +7744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72147712"/>
+        <c:axId val="98759424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7693,7 +7773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72133248"/>
+        <c:crossAx val="98749056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8009,11 +8089,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="71989888"/>
-        <c:axId val="71992064"/>
+        <c:axId val="98409088"/>
+        <c:axId val="98411264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71989888"/>
+        <c:axId val="98409088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8042,7 +8122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71992064"/>
+        <c:crossAx val="98411264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8050,7 +8130,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71992064"/>
+        <c:axId val="98411264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8080,7 +8160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71989888"/>
+        <c:crossAx val="98409088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8397,11 +8477,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72041216"/>
-        <c:axId val="72043136"/>
+        <c:axId val="98450048"/>
+        <c:axId val="98456320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72041216"/>
+        <c:axId val="98450048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8430,7 +8510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72043136"/>
+        <c:crossAx val="98456320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8438,7 +8518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72043136"/>
+        <c:axId val="98456320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8468,7 +8548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72041216"/>
+        <c:crossAx val="98450048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8785,11 +8865,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72078080"/>
-        <c:axId val="72080000"/>
+        <c:axId val="98493184"/>
+        <c:axId val="98495104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72078080"/>
+        <c:axId val="98493184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8818,7 +8898,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72080000"/>
+        <c:crossAx val="98495104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8826,7 +8906,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72080000"/>
+        <c:axId val="98495104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8856,7 +8936,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72078080"/>
+        <c:crossAx val="98493184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9180,11 +9260,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72434432"/>
-        <c:axId val="72436352"/>
+        <c:axId val="98538240"/>
+        <c:axId val="98540160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72434432"/>
+        <c:axId val="98538240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9213,7 +9293,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72436352"/>
+        <c:crossAx val="98540160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9221,7 +9301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72436352"/>
+        <c:axId val="98540160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9251,7 +9331,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72434432"/>
+        <c:crossAx val="98538240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9572,11 +9652,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72475392"/>
-        <c:axId val="72477312"/>
+        <c:axId val="98906880"/>
+        <c:axId val="98908800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72475392"/>
+        <c:axId val="98906880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9604,7 +9684,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72477312"/>
+        <c:crossAx val="98908800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9612,7 +9692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72477312"/>
+        <c:axId val="98908800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9641,7 +9721,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72475392"/>
+        <c:crossAx val="98906880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9957,11 +10037,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="72273920"/>
-        <c:axId val="72275840"/>
+        <c:axId val="98951552"/>
+        <c:axId val="98953472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72273920"/>
+        <c:axId val="98951552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9990,7 +10070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72275840"/>
+        <c:crossAx val="98953472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9998,7 +10078,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72275840"/>
+        <c:axId val="98953472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10028,7 +10108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72273920"/>
+        <c:crossAx val="98951552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10816,10 +10896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:S123"/>
+  <dimension ref="A4:S322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J23" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10827,7 +10907,7 @@
     <col min="1" max="1" width="53.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
   </cols>
@@ -10861,6 +10941,11 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>6813876</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -14109,7 +14194,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="113" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>1076.193186</v>
       </c>
@@ -14147,7 +14232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>503</v>
       </c>
@@ -14179,7 +14264,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B115">
         <v>257</v>
       </c>
@@ -14211,7 +14296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B116" s="1">
         <v>1795</v>
       </c>
@@ -14243,7 +14328,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B117" s="1">
         <v>1402810099</v>
       </c>
@@ -14281,7 +14366,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B118" s="1">
         <v>833710003</v>
       </c>
@@ -14331,7 +14416,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="119" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B119" s="1">
         <v>507077308</v>
       </c>
@@ -14381,7 +14466,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="120" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B120" s="1">
         <v>1414061707</v>
       </c>
@@ -14425,7 +14510,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>13</v>
       </c>
@@ -14469,7 +14554,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="122" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B122" s="1">
         <v>286649193</v>
       </c>
@@ -14507,7 +14592,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="123" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B123" s="1">
         <v>234441</v>
       </c>
@@ -14555,6 +14640,3361 @@
       </c>
       <c r="S123" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>4</v>
+      </c>
+      <c r="E129">
+        <v>8</v>
+      </c>
+      <c r="F129">
+        <v>16</v>
+      </c>
+      <c r="G129">
+        <v>32</v>
+      </c>
+      <c r="H129">
+        <v>64</v>
+      </c>
+      <c r="I129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>114</v>
+      </c>
+      <c r="B130" s="3">
+        <v>5676306</v>
+      </c>
+      <c r="C130" s="3">
+        <v>7713587</v>
+      </c>
+      <c r="D130" s="3">
+        <v>5624616</v>
+      </c>
+      <c r="E130" s="3">
+        <v>7905734</v>
+      </c>
+      <c r="F130" s="3">
+        <v>5846630</v>
+      </c>
+      <c r="G130" s="3">
+        <v>1403429</v>
+      </c>
+      <c r="H130" s="3">
+        <v>1434357</v>
+      </c>
+      <c r="I130" s="3">
+        <v>1308678</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>115</v>
+      </c>
+      <c r="B131" s="3">
+        <v>4173878</v>
+      </c>
+      <c r="C131" s="3">
+        <v>8488090</v>
+      </c>
+      <c r="D131" s="3">
+        <v>4190255</v>
+      </c>
+      <c r="E131" s="3">
+        <v>8486805</v>
+      </c>
+      <c r="F131" s="3">
+        <v>4198369</v>
+      </c>
+      <c r="G131" s="3">
+        <v>5159822</v>
+      </c>
+      <c r="H131" s="3">
+        <v>4212127</v>
+      </c>
+      <c r="I131" s="3">
+        <v>4237987</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>116</v>
+      </c>
+      <c r="B132" s="3">
+        <v>5749106</v>
+      </c>
+      <c r="C132" s="3">
+        <v>596</v>
+      </c>
+      <c r="D132" s="3">
+        <v>309</v>
+      </c>
+      <c r="E132" s="3">
+        <v>428</v>
+      </c>
+      <c r="F132" s="3">
+        <v>170</v>
+      </c>
+      <c r="G132" s="3">
+        <v>828</v>
+      </c>
+      <c r="H132" s="3">
+        <v>265</v>
+      </c>
+      <c r="I132" s="3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>117</v>
+      </c>
+      <c r="B133">
+        <v>6354110</v>
+      </c>
+      <c r="C133">
+        <v>9186313</v>
+      </c>
+      <c r="D133">
+        <v>6357069</v>
+      </c>
+      <c r="E133">
+        <v>7913894</v>
+      </c>
+      <c r="F133">
+        <v>7922126</v>
+      </c>
+      <c r="G133">
+        <v>7928292</v>
+      </c>
+      <c r="H133">
+        <v>7951841</v>
+      </c>
+      <c r="I133">
+        <v>6420306</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>118</v>
+      </c>
+      <c r="B134" s="3">
+        <v>5271718</v>
+      </c>
+      <c r="C134" s="3">
+        <v>755433</v>
+      </c>
+      <c r="D134" s="3">
+        <v>272426</v>
+      </c>
+      <c r="E134" s="3">
+        <v>134142</v>
+      </c>
+      <c r="F134" s="3">
+        <v>76196</v>
+      </c>
+      <c r="G134" s="3">
+        <v>38858</v>
+      </c>
+      <c r="H134" s="3">
+        <v>38212</v>
+      </c>
+      <c r="I134" s="3">
+        <v>20639</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>119</v>
+      </c>
+      <c r="B135" s="3">
+        <v>4911977</v>
+      </c>
+      <c r="C135" s="3">
+        <v>9179096</v>
+      </c>
+      <c r="D135" s="3">
+        <v>10887211</v>
+      </c>
+      <c r="E135" s="3">
+        <v>386831</v>
+      </c>
+      <c r="F135" s="3">
+        <v>314356</v>
+      </c>
+      <c r="G135" s="3">
+        <v>243227</v>
+      </c>
+      <c r="H135" s="3">
+        <v>268687</v>
+      </c>
+      <c r="I135" s="3">
+        <v>287168</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>120</v>
+      </c>
+      <c r="B136" s="3">
+        <v>4884973</v>
+      </c>
+      <c r="C136" s="3">
+        <v>6155533</v>
+      </c>
+      <c r="D136" s="3">
+        <v>6155231</v>
+      </c>
+      <c r="E136" s="3">
+        <v>6151533</v>
+      </c>
+      <c r="F136" s="3">
+        <v>6141856</v>
+      </c>
+      <c r="G136" s="3">
+        <v>6133294</v>
+      </c>
+      <c r="H136" s="3">
+        <v>6111459</v>
+      </c>
+      <c r="I136" s="3">
+        <v>6106350</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>121</v>
+      </c>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>125</v>
+      </c>
+      <c r="B138" s="3">
+        <v>6002304</v>
+      </c>
+      <c r="C138" s="3">
+        <v>1411687</v>
+      </c>
+      <c r="D138" s="3">
+        <v>7744597</v>
+      </c>
+      <c r="E138" s="3">
+        <v>718721</v>
+      </c>
+      <c r="F138" s="3">
+        <v>679587</v>
+      </c>
+      <c r="G138" s="3">
+        <v>371018</v>
+      </c>
+      <c r="H138" s="3">
+        <v>201441</v>
+      </c>
+      <c r="I138" s="3">
+        <v>249894</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>128</v>
+      </c>
+      <c r="B139" s="3">
+        <v>5169385</v>
+      </c>
+      <c r="C139" s="3">
+        <v>8991706</v>
+      </c>
+      <c r="D139" s="3">
+        <v>333701</v>
+      </c>
+      <c r="E139" s="3">
+        <v>149713</v>
+      </c>
+      <c r="F139" s="3">
+        <v>76997</v>
+      </c>
+      <c r="G139" s="3">
+        <v>60527</v>
+      </c>
+      <c r="H139" s="3">
+        <v>40744</v>
+      </c>
+      <c r="I139" s="3">
+        <v>23138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>131</v>
+      </c>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>134</v>
+      </c>
+      <c r="B141" s="3">
+        <v>7079323</v>
+      </c>
+      <c r="C141" s="3">
+        <v>10934388</v>
+      </c>
+      <c r="D141" s="3">
+        <v>777110</v>
+      </c>
+      <c r="E141" s="3">
+        <v>705884</v>
+      </c>
+      <c r="F141" s="3">
+        <v>703930</v>
+      </c>
+      <c r="G141" s="3">
+        <v>695054</v>
+      </c>
+      <c r="H141" s="3">
+        <v>505518</v>
+      </c>
+      <c r="I141" s="3">
+        <v>9481</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142" s="3">
+        <v>4943361</v>
+      </c>
+      <c r="C142" s="3">
+        <v>491493</v>
+      </c>
+      <c r="D142" s="3">
+        <v>498985</v>
+      </c>
+      <c r="E142" s="3">
+        <v>501298</v>
+      </c>
+      <c r="F142" s="3">
+        <v>484196</v>
+      </c>
+      <c r="G142" s="3">
+        <v>492453</v>
+      </c>
+      <c r="H142" s="3">
+        <v>478207</v>
+      </c>
+      <c r="I142" s="3">
+        <v>478593</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>2</v>
+      </c>
+      <c r="B143" s="3">
+        <v>9826165</v>
+      </c>
+      <c r="C143" s="3">
+        <v>10060263</v>
+      </c>
+      <c r="D143" s="3">
+        <v>9990896</v>
+      </c>
+      <c r="E143" s="3">
+        <v>10026881</v>
+      </c>
+      <c r="F143" s="3">
+        <v>10010618</v>
+      </c>
+      <c r="G143" s="3">
+        <v>10013748</v>
+      </c>
+      <c r="H143" s="3">
+        <v>10011278</v>
+      </c>
+      <c r="I143" s="3">
+        <v>9996153</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>9</v>
+      </c>
+      <c r="B144" s="3">
+        <v>14437602</v>
+      </c>
+      <c r="C144" s="3">
+        <v>1877</v>
+      </c>
+      <c r="D144" s="3">
+        <v>2501</v>
+      </c>
+      <c r="E144" s="3">
+        <v>2135</v>
+      </c>
+      <c r="F144" s="3">
+        <v>1256</v>
+      </c>
+      <c r="G144" s="3">
+        <v>1996</v>
+      </c>
+      <c r="H144" s="3">
+        <v>2093</v>
+      </c>
+      <c r="I144" s="3">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>110</v>
+      </c>
+      <c r="B145">
+        <v>9738834</v>
+      </c>
+      <c r="C145">
+        <v>11650039</v>
+      </c>
+      <c r="D145">
+        <v>11593920</v>
+      </c>
+      <c r="E145">
+        <v>11637199</v>
+      </c>
+      <c r="F145">
+        <v>11560531</v>
+      </c>
+      <c r="G145">
+        <v>11730086</v>
+      </c>
+      <c r="H145">
+        <v>11604913</v>
+      </c>
+      <c r="I145">
+        <v>11651960</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>106</v>
+      </c>
+      <c r="B146" s="3">
+        <v>9573092</v>
+      </c>
+      <c r="C146" s="3">
+        <v>7824295</v>
+      </c>
+      <c r="D146" s="3">
+        <v>5384550</v>
+      </c>
+      <c r="E146" s="3">
+        <v>4682752</v>
+      </c>
+      <c r="F146" s="3">
+        <v>4665796</v>
+      </c>
+      <c r="G146" s="3">
+        <v>4957293</v>
+      </c>
+      <c r="H146" s="3">
+        <v>4636598</v>
+      </c>
+      <c r="I146" s="3">
+        <v>3844912</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>111</v>
+      </c>
+      <c r="B147">
+        <v>10450999</v>
+      </c>
+      <c r="C147">
+        <v>8173969</v>
+      </c>
+      <c r="D147">
+        <v>5195173</v>
+      </c>
+      <c r="E147">
+        <v>5297516</v>
+      </c>
+      <c r="F147">
+        <v>4324595</v>
+      </c>
+      <c r="G147">
+        <v>5424441</v>
+      </c>
+      <c r="H147">
+        <v>5903481</v>
+      </c>
+      <c r="I147">
+        <v>5431571</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" s="3">
+        <v>10352425</v>
+      </c>
+      <c r="C148" s="3">
+        <v>10861201</v>
+      </c>
+      <c r="D148" s="3">
+        <v>10593044</v>
+      </c>
+      <c r="E148" s="3">
+        <v>10670844</v>
+      </c>
+      <c r="F148" s="3">
+        <v>10723988</v>
+      </c>
+      <c r="G148" s="3">
+        <v>10829917</v>
+      </c>
+      <c r="H148" s="3">
+        <v>10689442</v>
+      </c>
+      <c r="I148" s="3">
+        <v>10658002</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>122</v>
+      </c>
+      <c r="B149" s="3"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="3"/>
+      <c r="I149" s="3"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>124</v>
+      </c>
+      <c r="B150" s="3">
+        <v>10723921</v>
+      </c>
+      <c r="C150" s="3">
+        <v>8206118</v>
+      </c>
+      <c r="D150" s="3">
+        <v>5349723</v>
+      </c>
+      <c r="E150" s="3">
+        <v>5512366</v>
+      </c>
+      <c r="F150" s="3">
+        <v>5560398</v>
+      </c>
+      <c r="G150" s="3">
+        <v>4727827</v>
+      </c>
+      <c r="H150" s="3">
+        <v>5573792</v>
+      </c>
+      <c r="I150" s="3">
+        <v>5692459</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>127</v>
+      </c>
+      <c r="B151" s="3">
+        <v>9637339</v>
+      </c>
+      <c r="C151" s="3">
+        <v>8012164</v>
+      </c>
+      <c r="D151" s="3">
+        <v>3995404</v>
+      </c>
+      <c r="E151" s="3">
+        <v>4101948</v>
+      </c>
+      <c r="F151" s="3">
+        <v>3884708</v>
+      </c>
+      <c r="G151" s="3">
+        <v>3849270</v>
+      </c>
+      <c r="H151" s="3">
+        <v>3837262</v>
+      </c>
+      <c r="I151" s="3">
+        <v>4115422</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>130</v>
+      </c>
+      <c r="B152" s="3"/>
+      <c r="C152" s="3"/>
+      <c r="D152" s="3"/>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3"/>
+      <c r="H152" s="3"/>
+      <c r="I152" s="3"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>133</v>
+      </c>
+      <c r="B153" s="3">
+        <v>11985941</v>
+      </c>
+      <c r="C153" s="3">
+        <v>11070090</v>
+      </c>
+      <c r="D153" s="3">
+        <v>10684430</v>
+      </c>
+      <c r="E153" s="3">
+        <v>2229728</v>
+      </c>
+      <c r="F153" s="3">
+        <v>11003999</v>
+      </c>
+      <c r="G153" s="3">
+        <v>384394</v>
+      </c>
+      <c r="H153" s="3">
+        <v>10968950</v>
+      </c>
+      <c r="I153" s="3">
+        <v>372214</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>74</v>
+      </c>
+      <c r="B154" s="3">
+        <v>6806360</v>
+      </c>
+      <c r="C154" s="3">
+        <v>9375449</v>
+      </c>
+      <c r="D154" s="3">
+        <v>13799831</v>
+      </c>
+      <c r="E154" s="3">
+        <v>12598141</v>
+      </c>
+      <c r="F154" s="3">
+        <v>8845517</v>
+      </c>
+      <c r="G154" s="3">
+        <v>11521466</v>
+      </c>
+      <c r="H154" s="3">
+        <v>7997701</v>
+      </c>
+      <c r="I154" s="3">
+        <v>5510868</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>69</v>
+      </c>
+      <c r="B155" s="3">
+        <v>5781194</v>
+      </c>
+      <c r="C155" s="3">
+        <v>5920512</v>
+      </c>
+      <c r="D155" s="3">
+        <v>11044722</v>
+      </c>
+      <c r="E155" s="3">
+        <v>8168633</v>
+      </c>
+      <c r="F155" s="3">
+        <v>5918903</v>
+      </c>
+      <c r="G155" s="3">
+        <v>5930554</v>
+      </c>
+      <c r="H155" s="3">
+        <v>7345864</v>
+      </c>
+      <c r="I155" s="3">
+        <v>7469493</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>70</v>
+      </c>
+      <c r="B156" s="3">
+        <v>7502169</v>
+      </c>
+      <c r="C156" s="3">
+        <v>593</v>
+      </c>
+      <c r="D156" s="3">
+        <v>286</v>
+      </c>
+      <c r="E156" s="3">
+        <v>246</v>
+      </c>
+      <c r="F156" s="3">
+        <v>227</v>
+      </c>
+      <c r="G156" s="3">
+        <v>347</v>
+      </c>
+      <c r="H156" s="3">
+        <v>286</v>
+      </c>
+      <c r="I156" s="3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>71</v>
+      </c>
+      <c r="B157">
+        <v>6395740</v>
+      </c>
+      <c r="C157">
+        <v>11892896</v>
+      </c>
+      <c r="D157">
+        <v>6404216</v>
+      </c>
+      <c r="E157">
+        <v>6386009</v>
+      </c>
+      <c r="F157">
+        <v>8111637</v>
+      </c>
+      <c r="G157">
+        <v>8132967</v>
+      </c>
+      <c r="H157">
+        <v>6396520</v>
+      </c>
+      <c r="I157">
+        <v>8277906</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>109</v>
+      </c>
+      <c r="B158" s="3">
+        <v>6147457</v>
+      </c>
+      <c r="C158" s="3">
+        <v>6322449</v>
+      </c>
+      <c r="D158" s="3">
+        <v>7482088</v>
+      </c>
+      <c r="E158" s="3">
+        <v>717178</v>
+      </c>
+      <c r="F158" s="3">
+        <v>646505</v>
+      </c>
+      <c r="G158" s="3">
+        <v>522916</v>
+      </c>
+      <c r="H158" s="3">
+        <v>207519</v>
+      </c>
+      <c r="I158" s="3">
+        <v>91308</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>112</v>
+      </c>
+      <c r="B159" s="3">
+        <v>6056448</v>
+      </c>
+      <c r="C159" s="3">
+        <v>2409783</v>
+      </c>
+      <c r="D159" s="3">
+        <v>5430664</v>
+      </c>
+      <c r="E159" s="3">
+        <v>1254737</v>
+      </c>
+      <c r="F159" s="3">
+        <v>1304162</v>
+      </c>
+      <c r="G159" s="3">
+        <v>1332186</v>
+      </c>
+      <c r="H159" s="3">
+        <v>1011383</v>
+      </c>
+      <c r="I159" s="3">
+        <v>480224</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>72</v>
+      </c>
+      <c r="B160" s="3">
+        <v>6133023</v>
+      </c>
+      <c r="C160" s="3">
+        <v>12102300</v>
+      </c>
+      <c r="D160" s="3">
+        <v>7771889</v>
+      </c>
+      <c r="E160" s="3">
+        <v>7751134</v>
+      </c>
+      <c r="F160" s="3">
+        <v>7827144</v>
+      </c>
+      <c r="G160" s="3">
+        <v>7716848</v>
+      </c>
+      <c r="H160" s="3">
+        <v>7759021</v>
+      </c>
+      <c r="I160" s="3">
+        <v>7867672</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>123</v>
+      </c>
+      <c r="B161" s="3"/>
+      <c r="C161" s="3"/>
+      <c r="D161" s="3"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="G161" s="3"/>
+      <c r="H161" s="3"/>
+      <c r="I161" s="3"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>126</v>
+      </c>
+      <c r="B162" s="3">
+        <v>6094953</v>
+      </c>
+      <c r="C162" s="3">
+        <v>9504428</v>
+      </c>
+      <c r="D162" s="3">
+        <v>6466773</v>
+      </c>
+      <c r="E162" s="3">
+        <v>6162666</v>
+      </c>
+      <c r="F162" s="3">
+        <v>1955323</v>
+      </c>
+      <c r="G162" s="3">
+        <v>1666677</v>
+      </c>
+      <c r="H162" s="3">
+        <v>1824917</v>
+      </c>
+      <c r="I162" s="3">
+        <v>735779</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>129</v>
+      </c>
+      <c r="B163" s="3">
+        <v>6375781</v>
+      </c>
+      <c r="C163" s="3">
+        <v>7945662</v>
+      </c>
+      <c r="D163" s="3">
+        <v>12200556</v>
+      </c>
+      <c r="E163" s="3">
+        <v>6036337</v>
+      </c>
+      <c r="F163" s="3">
+        <v>573693</v>
+      </c>
+      <c r="G163" s="3">
+        <v>341814</v>
+      </c>
+      <c r="H163" s="3">
+        <v>131824</v>
+      </c>
+      <c r="I163" s="3">
+        <v>84045</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>132</v>
+      </c>
+      <c r="B164" s="3"/>
+      <c r="C164" s="3"/>
+      <c r="D164" s="3"/>
+      <c r="E164" s="3"/>
+      <c r="F164" s="3"/>
+      <c r="G164" s="3"/>
+      <c r="H164" s="3"/>
+      <c r="I164" s="3"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>135</v>
+      </c>
+      <c r="B165" s="3">
+        <v>7576736</v>
+      </c>
+      <c r="C165" s="3">
+        <v>12820925</v>
+      </c>
+      <c r="D165" s="3">
+        <v>9780267</v>
+      </c>
+      <c r="E165" s="3">
+        <v>1884530</v>
+      </c>
+      <c r="F165" s="3">
+        <v>1982678</v>
+      </c>
+      <c r="G165" s="3">
+        <v>2033</v>
+      </c>
+      <c r="H165" s="3">
+        <v>2275</v>
+      </c>
+      <c r="I165" s="3">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>43</v>
+      </c>
+      <c r="B168">
+        <v>291678068575</v>
+      </c>
+      <c r="C168" t="s">
+        <v>20</v>
+      </c>
+      <c r="E168" t="s">
+        <v>75</v>
+      </c>
+      <c r="F168">
+        <v>26829298828</v>
+      </c>
+      <c r="G168" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>27026065319</v>
+      </c>
+      <c r="C169" t="s">
+        <v>30</v>
+      </c>
+      <c r="F169">
+        <v>16724380191</v>
+      </c>
+      <c r="G169" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>55899684</v>
+      </c>
+      <c r="C170" t="s">
+        <v>137</v>
+      </c>
+      <c r="F170">
+        <v>20932682</v>
+      </c>
+      <c r="G170" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>22463344</v>
+      </c>
+      <c r="C171" t="s">
+        <v>138</v>
+      </c>
+      <c r="D171">
+        <f>B171/B170 * 100</f>
+        <v>40.185100151907839</v>
+      </c>
+      <c r="F171">
+        <v>9259519</v>
+      </c>
+      <c r="G171" t="s">
+        <v>138</v>
+      </c>
+      <c r="H171">
+        <f>F171/F170 * 100</f>
+        <v>44.234747367776379</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>9245008504</v>
+      </c>
+      <c r="C172" t="s">
+        <v>37</v>
+      </c>
+      <c r="F172">
+        <v>3954122463</v>
+      </c>
+      <c r="G172" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B173">
+        <v>7583573</v>
+      </c>
+      <c r="C173" t="s">
+        <v>39</v>
+      </c>
+      <c r="F173">
+        <v>5028398</v>
+      </c>
+      <c r="G173" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B174">
+        <v>20689657820</v>
+      </c>
+      <c r="C174" t="s">
+        <v>139</v>
+      </c>
+      <c r="F174">
+        <v>1839664107</v>
+      </c>
+      <c r="G174" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>811</v>
+      </c>
+      <c r="C175" t="s">
+        <v>140</v>
+      </c>
+      <c r="F175">
+        <v>810</v>
+      </c>
+      <c r="G175" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B176">
+        <v>156659.36922200001</v>
+      </c>
+      <c r="C176" t="s">
+        <v>141</v>
+      </c>
+      <c r="F176">
+        <v>14292.175730000001</v>
+      </c>
+      <c r="G176" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>156660.63276400001</v>
+      </c>
+      <c r="C177" t="s">
+        <v>12</v>
+      </c>
+      <c r="F177">
+        <v>14293.603504000001</v>
+      </c>
+      <c r="G177" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>276526511601</v>
+      </c>
+      <c r="C178" t="s">
+        <v>23</v>
+      </c>
+      <c r="D178">
+        <f>B178/B168 * 100</f>
+        <v>94.805383535339743</v>
+      </c>
+      <c r="F178">
+        <v>20147735002</v>
+      </c>
+      <c r="G178" t="s">
+        <v>23</v>
+      </c>
+      <c r="H178">
+        <f>F178/F168 * 100</f>
+        <v>75.096017719900729</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>191972396985</v>
+      </c>
+      <c r="C179" t="s">
+        <v>27</v>
+      </c>
+      <c r="D179">
+        <f>B179/B168 * 100</f>
+        <v>65.816534620818629</v>
+      </c>
+      <c r="F179">
+        <v>13465580402</v>
+      </c>
+      <c r="G179" t="s">
+        <v>27</v>
+      </c>
+      <c r="H179">
+        <f>F179/F168 * 100</f>
+        <v>50.189833466489432</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>142</v>
+      </c>
+      <c r="B181">
+        <v>10197151086</v>
+      </c>
+      <c r="C181" t="s">
+        <v>20</v>
+      </c>
+      <c r="E181" t="s">
+        <v>82</v>
+      </c>
+      <c r="F181">
+        <v>13732922235</v>
+      </c>
+      <c r="G181" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B182">
+        <v>9060697991</v>
+      </c>
+      <c r="C182" t="s">
+        <v>30</v>
+      </c>
+      <c r="F182">
+        <v>12350808053</v>
+      </c>
+      <c r="G182" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B183">
+        <v>1964406</v>
+      </c>
+      <c r="C183" t="s">
+        <v>137</v>
+      </c>
+      <c r="F183">
+        <v>1797505</v>
+      </c>
+      <c r="G183" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B184">
+        <v>755138</v>
+      </c>
+      <c r="C184" t="s">
+        <v>138</v>
+      </c>
+      <c r="D184">
+        <f>B184/B183 * 100</f>
+        <v>38.441035101705047</v>
+      </c>
+      <c r="F184">
+        <v>643599</v>
+      </c>
+      <c r="G184" t="s">
+        <v>138</v>
+      </c>
+      <c r="H184">
+        <f>F184/F183 * 100</f>
+        <v>35.805129888373052</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>1688643722</v>
+      </c>
+      <c r="C185" t="s">
+        <v>37</v>
+      </c>
+      <c r="F185">
+        <v>2222362942</v>
+      </c>
+      <c r="G185" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B186">
+        <v>1378536</v>
+      </c>
+      <c r="C186" t="s">
+        <v>39</v>
+      </c>
+      <c r="F186">
+        <v>1152892</v>
+      </c>
+      <c r="G186" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B187">
+        <v>1066066047</v>
+      </c>
+      <c r="C187" t="s">
+        <v>139</v>
+      </c>
+      <c r="F187">
+        <v>1071409693</v>
+      </c>
+      <c r="G187" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B188">
+        <v>813</v>
+      </c>
+      <c r="C188" t="s">
+        <v>140</v>
+      </c>
+      <c r="F188">
+        <v>811</v>
+      </c>
+      <c r="G188" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B189">
+        <v>8568.5000070000006</v>
+      </c>
+      <c r="C189" t="s">
+        <v>141</v>
+      </c>
+      <c r="F189">
+        <v>8162.8342249999996</v>
+      </c>
+      <c r="G189" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B190">
+        <v>8571.7451239999991</v>
+      </c>
+      <c r="C190" t="s">
+        <v>12</v>
+      </c>
+      <c r="F190">
+        <v>8164.1139730000004</v>
+      </c>
+      <c r="G190" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B191">
+        <v>6384758343</v>
+      </c>
+      <c r="C191" t="s">
+        <v>23</v>
+      </c>
+      <c r="D191">
+        <f>B191/B181 * 100</f>
+        <v>62.613158215982914</v>
+      </c>
+      <c r="F191">
+        <v>8452488987</v>
+      </c>
+      <c r="G191" t="s">
+        <v>23</v>
+      </c>
+      <c r="H191">
+        <f>F191/F181 * 100</f>
+        <v>61.549092337083344</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B192">
+        <v>4754795265</v>
+      </c>
+      <c r="C192" t="s">
+        <v>27</v>
+      </c>
+      <c r="D192">
+        <f>B192/B181 * 100</f>
+        <v>46.628663485510309</v>
+      </c>
+      <c r="F192">
+        <v>5866968288</v>
+      </c>
+      <c r="G192" t="s">
+        <v>27</v>
+      </c>
+      <c r="H192">
+        <f>F192/F181 * 100</f>
+        <v>42.721921726515916</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>143</v>
+      </c>
+      <c r="B194">
+        <v>283745513479</v>
+      </c>
+      <c r="C194" t="s">
+        <v>20</v>
+      </c>
+      <c r="E194" t="s">
+        <v>144</v>
+      </c>
+      <c r="F194">
+        <v>152143420476</v>
+      </c>
+      <c r="G194" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B195">
+        <v>25954485320</v>
+      </c>
+      <c r="C195" t="s">
+        <v>30</v>
+      </c>
+      <c r="F195">
+        <v>84084784848</v>
+      </c>
+      <c r="G195" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B196">
+        <v>52064857</v>
+      </c>
+      <c r="C196" t="s">
+        <v>137</v>
+      </c>
+      <c r="F196">
+        <v>182817391</v>
+      </c>
+      <c r="G196" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B197">
+        <v>28690612</v>
+      </c>
+      <c r="C197" t="s">
+        <v>138</v>
+      </c>
+      <c r="D197">
+        <f>B197/B196 * 100</f>
+        <v>55.105523481990936</v>
+      </c>
+      <c r="F197">
+        <v>86619973</v>
+      </c>
+      <c r="G197" t="s">
+        <v>138</v>
+      </c>
+      <c r="H197">
+        <f>F197/F196 * 100</f>
+        <v>47.38059794322303</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B198">
+        <v>5337113446</v>
+      </c>
+      <c r="C198" t="s">
+        <v>37</v>
+      </c>
+      <c r="F198">
+        <v>16839694666</v>
+      </c>
+      <c r="G198" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B199">
+        <v>7444252</v>
+      </c>
+      <c r="C199" t="s">
+        <v>39</v>
+      </c>
+      <c r="F199">
+        <v>43980907</v>
+      </c>
+      <c r="G199" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B200">
+        <v>18355120628</v>
+      </c>
+      <c r="C200" t="s">
+        <v>139</v>
+      </c>
+      <c r="F200">
+        <v>8585156031</v>
+      </c>
+      <c r="G200" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B201">
+        <v>812</v>
+      </c>
+      <c r="C201" t="s">
+        <v>140</v>
+      </c>
+      <c r="F201">
+        <v>810</v>
+      </c>
+      <c r="G201" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B202">
+        <v>139045.205594</v>
+      </c>
+      <c r="C202" t="s">
+        <v>141</v>
+      </c>
+      <c r="F202">
+        <v>64997.364043000001</v>
+      </c>
+      <c r="G202" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B203">
+        <v>139045.46944300001</v>
+      </c>
+      <c r="C203" t="s">
+        <v>12</v>
+      </c>
+      <c r="F203">
+        <v>64997.523718999997</v>
+      </c>
+      <c r="G203" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B204">
+        <v>271580354630</v>
+      </c>
+      <c r="C204" t="s">
+        <v>23</v>
+      </c>
+      <c r="D204">
+        <f>B204/B194 * 100</f>
+        <v>95.712651558841173</v>
+      </c>
+      <c r="F204">
+        <v>117184865731</v>
+      </c>
+      <c r="G204" t="s">
+        <v>23</v>
+      </c>
+      <c r="H204">
+        <f>F204/F194 * 100</f>
+        <v>77.02263125436005</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B205">
+        <v>165240064931</v>
+      </c>
+      <c r="C205" t="s">
+        <v>27</v>
+      </c>
+      <c r="D205">
+        <f>B205/B194 * 100</f>
+        <v>58.235304905791722</v>
+      </c>
+      <c r="F205">
+        <v>63505196962</v>
+      </c>
+      <c r="G205" t="s">
+        <v>27</v>
+      </c>
+      <c r="H205">
+        <f>F205/F194 * 100</f>
+        <v>41.74035049515512</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>145</v>
+      </c>
+      <c r="B207">
+        <v>11274354575</v>
+      </c>
+      <c r="C207" t="s">
+        <v>20</v>
+      </c>
+      <c r="E207" t="s">
+        <v>146</v>
+      </c>
+      <c r="F207">
+        <v>14141779952</v>
+      </c>
+      <c r="G207" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B208">
+        <v>11479457017</v>
+      </c>
+      <c r="C208" t="s">
+        <v>30</v>
+      </c>
+      <c r="F208">
+        <v>14137753562</v>
+      </c>
+      <c r="G208" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>1211026</v>
+      </c>
+      <c r="C209" t="s">
+        <v>137</v>
+      </c>
+      <c r="F209">
+        <v>1569371</v>
+      </c>
+      <c r="G209" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>267876</v>
+      </c>
+      <c r="C210" t="s">
+        <v>138</v>
+      </c>
+      <c r="D210">
+        <f>B210/B209 * 100</f>
+        <v>22.119756305810114</v>
+      </c>
+      <c r="F210">
+        <v>465757</v>
+      </c>
+      <c r="G210" t="s">
+        <v>138</v>
+      </c>
+      <c r="H210">
+        <f>F210/F209 * 100</f>
+        <v>29.677941034975159</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>2326287379</v>
+      </c>
+      <c r="C211" t="s">
+        <v>37</v>
+      </c>
+      <c r="F211">
+        <v>2766338836</v>
+      </c>
+      <c r="G211" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>163365</v>
+      </c>
+      <c r="C212" t="s">
+        <v>39</v>
+      </c>
+      <c r="F212">
+        <v>322730</v>
+      </c>
+      <c r="G212" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>1056288556</v>
+      </c>
+      <c r="C213" t="s">
+        <v>139</v>
+      </c>
+      <c r="F213">
+        <v>1061139985</v>
+      </c>
+      <c r="G213" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>812</v>
+      </c>
+      <c r="C214" t="s">
+        <v>140</v>
+      </c>
+      <c r="F214">
+        <v>811</v>
+      </c>
+      <c r="G214" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>8044.6088380000001</v>
+      </c>
+      <c r="C215" t="s">
+        <v>141</v>
+      </c>
+      <c r="F215">
+        <v>8019.6252960000002</v>
+      </c>
+      <c r="G215" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>8044.8160479999997</v>
+      </c>
+      <c r="C216" t="s">
+        <v>12</v>
+      </c>
+      <c r="F216">
+        <v>8019.816675</v>
+      </c>
+      <c r="G216" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>6463660745</v>
+      </c>
+      <c r="C217" t="s">
+        <v>23</v>
+      </c>
+      <c r="D217">
+        <f>B217/B207 * 100</f>
+        <v>57.330649856734709</v>
+      </c>
+      <c r="F217">
+        <v>8179511829</v>
+      </c>
+      <c r="G217" t="s">
+        <v>23</v>
+      </c>
+      <c r="H217">
+        <f>F217/F207 * 100</f>
+        <v>57.839337457964149</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>3904277650</v>
+      </c>
+      <c r="C218" t="s">
+        <v>27</v>
+      </c>
+      <c r="D218">
+        <f>B218/B207 * 100</f>
+        <v>34.629722030008089</v>
+      </c>
+      <c r="F218">
+        <v>5025035784</v>
+      </c>
+      <c r="G218" t="s">
+        <v>27</v>
+      </c>
+      <c r="H218">
+        <f>F218/F207 * 100</f>
+        <v>35.533262439777495</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>147</v>
+      </c>
+      <c r="B220">
+        <v>376249952235</v>
+      </c>
+      <c r="C220" t="s">
+        <v>20</v>
+      </c>
+      <c r="E220" t="s">
+        <v>94</v>
+      </c>
+      <c r="F220">
+        <v>153488898798</v>
+      </c>
+      <c r="G220" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>7624996538</v>
+      </c>
+      <c r="C221" t="s">
+        <v>30</v>
+      </c>
+      <c r="F221">
+        <v>8195210791</v>
+      </c>
+      <c r="G221" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>44550638</v>
+      </c>
+      <c r="C222" t="s">
+        <v>137</v>
+      </c>
+      <c r="F222">
+        <v>103279246</v>
+      </c>
+      <c r="G222" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>34565580</v>
+      </c>
+      <c r="C223" t="s">
+        <v>138</v>
+      </c>
+      <c r="D223">
+        <f>B223/B222 * 100</f>
+        <v>77.587171703354727</v>
+      </c>
+      <c r="F223">
+        <v>58097662</v>
+      </c>
+      <c r="G223" t="s">
+        <v>138</v>
+      </c>
+      <c r="H223">
+        <f>F223/F222 * 100</f>
+        <v>56.252988136648483</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>1294512738</v>
+      </c>
+      <c r="C224" t="s">
+        <v>37</v>
+      </c>
+      <c r="F224">
+        <v>1473734160</v>
+      </c>
+      <c r="G224" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>2692273</v>
+      </c>
+      <c r="C225" t="s">
+        <v>39</v>
+      </c>
+      <c r="F225">
+        <v>4820628</v>
+      </c>
+      <c r="G225" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>24345728260</v>
+      </c>
+      <c r="C226" t="s">
+        <v>139</v>
+      </c>
+      <c r="F226">
+        <v>8826103713</v>
+      </c>
+      <c r="G226" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>812</v>
+      </c>
+      <c r="C227" t="s">
+        <v>140</v>
+      </c>
+      <c r="F227">
+        <v>810</v>
+      </c>
+      <c r="G227" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>184643.57956799999</v>
+      </c>
+      <c r="C228" t="s">
+        <v>141</v>
+      </c>
+      <c r="F228">
+        <v>66780.231138999996</v>
+      </c>
+      <c r="G228" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>184643.49950500001</v>
+      </c>
+      <c r="C229" t="s">
+        <v>12</v>
+      </c>
+      <c r="F229">
+        <v>66780.386148999998</v>
+      </c>
+      <c r="G229" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>373088624137</v>
+      </c>
+      <c r="C230" t="s">
+        <v>23</v>
+      </c>
+      <c r="D230">
+        <f>B230/B220 * 100</f>
+        <v>99.159779800842202</v>
+      </c>
+      <c r="F230">
+        <v>150038824661</v>
+      </c>
+      <c r="G230" t="s">
+        <v>23</v>
+      </c>
+      <c r="H230">
+        <f>F230/F220 * 100</f>
+        <v>97.752232139250353</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>316318256658</v>
+      </c>
+      <c r="C231" t="s">
+        <v>27</v>
+      </c>
+      <c r="D231">
+        <f>B231/B220 * 100</f>
+        <v>84.071308123497758</v>
+      </c>
+      <c r="F231">
+        <v>130359824536</v>
+      </c>
+      <c r="G231" t="s">
+        <v>27</v>
+      </c>
+      <c r="H231">
+        <f>F231/F220 * 100</f>
+        <v>84.931109387631238</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>148</v>
+      </c>
+      <c r="B233">
+        <v>13241630079</v>
+      </c>
+      <c r="C233" t="s">
+        <v>20</v>
+      </c>
+      <c r="E233" t="s">
+        <v>149</v>
+      </c>
+      <c r="F233">
+        <v>13558533770</v>
+      </c>
+      <c r="G233" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>11796230989</v>
+      </c>
+      <c r="C234" t="s">
+        <v>30</v>
+      </c>
+      <c r="F234">
+        <v>11994026068</v>
+      </c>
+      <c r="G234" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>1398970</v>
+      </c>
+      <c r="C235" t="s">
+        <v>137</v>
+      </c>
+      <c r="F235">
+        <v>895529</v>
+      </c>
+      <c r="G235" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>366870</v>
+      </c>
+      <c r="C236" t="s">
+        <v>138</v>
+      </c>
+      <c r="D236">
+        <f>B236/B235 * 100</f>
+        <v>26.224293587425034</v>
+      </c>
+      <c r="F236">
+        <v>265083</v>
+      </c>
+      <c r="G236" t="s">
+        <v>138</v>
+      </c>
+      <c r="H236">
+        <f>F236/F235 * 100</f>
+        <v>29.600716448043556</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>2275543676</v>
+      </c>
+      <c r="C237" t="s">
+        <v>37</v>
+      </c>
+      <c r="F237">
+        <v>2293858178</v>
+      </c>
+      <c r="G237" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>281197</v>
+      </c>
+      <c r="C238" t="s">
+        <v>39</v>
+      </c>
+      <c r="F238">
+        <v>421693</v>
+      </c>
+      <c r="G238" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>1062668058</v>
+      </c>
+      <c r="C239" t="s">
+        <v>139</v>
+      </c>
+      <c r="F239">
+        <v>1060293427</v>
+      </c>
+      <c r="G239" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>812</v>
+      </c>
+      <c r="C240" t="s">
+        <v>140</v>
+      </c>
+      <c r="F240">
+        <v>810</v>
+      </c>
+      <c r="G240" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>8056.6675770000002</v>
+      </c>
+      <c r="C241" t="s">
+        <v>141</v>
+      </c>
+      <c r="F241">
+        <v>8043.2529489999997</v>
+      </c>
+      <c r="G241" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>8056.910715</v>
+      </c>
+      <c r="C242" t="s">
+        <v>12</v>
+      </c>
+      <c r="F242">
+        <v>8043.2218210000001</v>
+      </c>
+      <c r="G242" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>8139161639</v>
+      </c>
+      <c r="C243" t="s">
+        <v>23</v>
+      </c>
+      <c r="D243">
+        <f>B243/B233 * 100</f>
+        <v>61.466462893476816</v>
+      </c>
+      <c r="F243">
+        <v>8288328221</v>
+      </c>
+      <c r="G243" t="s">
+        <v>23</v>
+      </c>
+      <c r="H243">
+        <f>F243/F233 * 100</f>
+        <v>61.129974388078686</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>6309134924</v>
+      </c>
+      <c r="C244" t="s">
+        <v>27</v>
+      </c>
+      <c r="D244">
+        <f>B244/B233 * 100</f>
+        <v>47.646210371075867</v>
+      </c>
+      <c r="F244">
+        <v>5983836892</v>
+      </c>
+      <c r="G244" t="s">
+        <v>27</v>
+      </c>
+      <c r="H244">
+        <f>F244/F233 * 100</f>
+        <v>44.133362747821664</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>150</v>
+      </c>
+      <c r="B246">
+        <v>1259730786</v>
+      </c>
+      <c r="C246" t="s">
+        <v>20</v>
+      </c>
+      <c r="E246" t="s">
+        <v>99</v>
+      </c>
+      <c r="F246">
+        <v>1609188165</v>
+      </c>
+      <c r="G246" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>1201707563</v>
+      </c>
+      <c r="C247" t="s">
+        <v>30</v>
+      </c>
+      <c r="F247">
+        <v>1547849324</v>
+      </c>
+      <c r="G247" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>1307399</v>
+      </c>
+      <c r="C248" t="s">
+        <v>137</v>
+      </c>
+      <c r="F248">
+        <v>1736529</v>
+      </c>
+      <c r="G248" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B249">
+        <v>294932</v>
+      </c>
+      <c r="C249" t="s">
+        <v>138</v>
+      </c>
+      <c r="D249">
+        <f>B249/B248 * 100</f>
+        <v>22.558683309379919</v>
+      </c>
+      <c r="F249">
+        <v>669410</v>
+      </c>
+      <c r="G249" t="s">
+        <v>138</v>
+      </c>
+      <c r="H249">
+        <f>F249/F248 * 100</f>
+        <v>38.548737164769491</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B250">
+        <v>254475335</v>
+      </c>
+      <c r="C250" t="s">
+        <v>37</v>
+      </c>
+      <c r="F250">
+        <v>325869389</v>
+      </c>
+      <c r="G250" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>237507</v>
+      </c>
+      <c r="C251" t="s">
+        <v>39</v>
+      </c>
+      <c r="F251">
+        <v>428101</v>
+      </c>
+      <c r="G251" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B252">
+        <v>139356399</v>
+      </c>
+      <c r="C252" t="s">
+        <v>139</v>
+      </c>
+      <c r="F252">
+        <v>136689711</v>
+      </c>
+      <c r="G252" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B253">
+        <v>813</v>
+      </c>
+      <c r="C253" t="s">
+        <v>140</v>
+      </c>
+      <c r="F253">
+        <v>811</v>
+      </c>
+      <c r="G253" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B254">
+        <v>1073.4383339999999</v>
+      </c>
+      <c r="C254" t="s">
+        <v>141</v>
+      </c>
+      <c r="F254">
+        <v>1049.037497</v>
+      </c>
+      <c r="G254" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B255">
+        <v>1073.8579380000001</v>
+      </c>
+      <c r="C255" t="s">
+        <v>12</v>
+      </c>
+      <c r="F255">
+        <v>1049.469486</v>
+      </c>
+      <c r="G255" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B256">
+        <v>757321416</v>
+      </c>
+      <c r="C256" t="s">
+        <v>23</v>
+      </c>
+      <c r="D256">
+        <f>B256/B246 * 100</f>
+        <v>60.11771915209826</v>
+      </c>
+      <c r="F256">
+        <v>978273921</v>
+      </c>
+      <c r="G256" t="s">
+        <v>23</v>
+      </c>
+      <c r="H256">
+        <f>F256/F246 * 100</f>
+        <v>60.793009933676714</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B257">
+        <v>507775250</v>
+      </c>
+      <c r="C257" t="s">
+        <v>27</v>
+      </c>
+      <c r="D257">
+        <f>B257/B246 * 100</f>
+        <v>40.308235350215533</v>
+      </c>
+      <c r="F257">
+        <v>579323144</v>
+      </c>
+      <c r="G257" t="s">
+        <v>27</v>
+      </c>
+      <c r="H257">
+        <f>F257/F246 * 100</f>
+        <v>36.000957290162525</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>151</v>
+      </c>
+      <c r="B259">
+        <v>269563013244</v>
+      </c>
+      <c r="C259" t="s">
+        <v>20</v>
+      </c>
+      <c r="E259" t="s">
+        <v>152</v>
+      </c>
+      <c r="F259">
+        <v>141304314234</v>
+      </c>
+      <c r="G259" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B260">
+        <v>9293327135</v>
+      </c>
+      <c r="C260" t="s">
+        <v>30</v>
+      </c>
+      <c r="F260">
+        <v>42315917082</v>
+      </c>
+      <c r="G260" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B261">
+        <v>48539719</v>
+      </c>
+      <c r="C261" t="s">
+        <v>137</v>
+      </c>
+      <c r="F261">
+        <v>95948521</v>
+      </c>
+      <c r="G261" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B262">
+        <v>20532961</v>
+      </c>
+      <c r="C262" t="s">
+        <v>138</v>
+      </c>
+      <c r="D262">
+        <f>B262/B261 * 100</f>
+        <v>42.301359428965789</v>
+      </c>
+      <c r="F262">
+        <v>45100016</v>
+      </c>
+      <c r="G262" t="s">
+        <v>138</v>
+      </c>
+      <c r="H262">
+        <f>F262/F261 * 100</f>
+        <v>47.004388947277256</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B263">
+        <v>2055443160</v>
+      </c>
+      <c r="C263" t="s">
+        <v>37</v>
+      </c>
+      <c r="F263">
+        <v>9568523775</v>
+      </c>
+      <c r="G263" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B264">
+        <v>6552759</v>
+      </c>
+      <c r="C264" t="s">
+        <v>39</v>
+      </c>
+      <c r="F264">
+        <v>14873153</v>
+      </c>
+      <c r="G264" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B265">
+        <v>17005574764</v>
+      </c>
+      <c r="C265" t="s">
+        <v>139</v>
+      </c>
+      <c r="F265">
+        <v>8182475544</v>
+      </c>
+      <c r="G265" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B266">
+        <v>812</v>
+      </c>
+      <c r="C266" t="s">
+        <v>140</v>
+      </c>
+      <c r="F266">
+        <v>809</v>
+      </c>
+      <c r="G266" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B267">
+        <v>128829.395018</v>
+      </c>
+      <c r="C267" t="s">
+        <v>141</v>
+      </c>
+      <c r="F267">
+        <v>61963.139481999999</v>
+      </c>
+      <c r="G267" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B268">
+        <v>128829.458683</v>
+      </c>
+      <c r="C268" t="s">
+        <v>12</v>
+      </c>
+      <c r="F268">
+        <v>61963.308987999997</v>
+      </c>
+      <c r="G268" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B269">
+        <v>265028205577</v>
+      </c>
+      <c r="C269" t="s">
+        <v>23</v>
+      </c>
+      <c r="D269">
+        <f>B269/B259 * 100</f>
+        <v>98.317718884194534</v>
+      </c>
+      <c r="F269">
+        <v>123512261869</v>
+      </c>
+      <c r="G269" t="s">
+        <v>23</v>
+      </c>
+      <c r="H269">
+        <f>F269/F259 * 100</f>
+        <v>87.408698409918074</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B270">
+        <v>230033953882</v>
+      </c>
+      <c r="C270" t="s">
+        <v>27</v>
+      </c>
+      <c r="D270">
+        <f>B270/B259 * 100</f>
+        <v>85.335874203847268</v>
+      </c>
+      <c r="F270">
+        <v>83954365068</v>
+      </c>
+      <c r="G270" t="s">
+        <v>27</v>
+      </c>
+      <c r="H270">
+        <f>F270/F259 * 100</f>
+        <v>59.413872480193021</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>153</v>
+      </c>
+      <c r="B272">
+        <v>211298869098</v>
+      </c>
+      <c r="C272" t="s">
+        <v>20</v>
+      </c>
+      <c r="E272" t="s">
+        <v>154</v>
+      </c>
+      <c r="F272">
+        <v>380148816157</v>
+      </c>
+      <c r="G272" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B273">
+        <v>87231790846</v>
+      </c>
+      <c r="C273" t="s">
+        <v>30</v>
+      </c>
+      <c r="F273">
+        <v>95159695374</v>
+      </c>
+      <c r="G273" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B274">
+        <v>57359724</v>
+      </c>
+      <c r="C274" t="s">
+        <v>137</v>
+      </c>
+      <c r="F274">
+        <v>69807415</v>
+      </c>
+      <c r="G274" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B275">
+        <v>25525686</v>
+      </c>
+      <c r="C275" t="s">
+        <v>138</v>
+      </c>
+      <c r="D275">
+        <f>B275/B274 * 100</f>
+        <v>44.501061406780828</v>
+      </c>
+      <c r="F275">
+        <v>30596614</v>
+      </c>
+      <c r="G275" t="s">
+        <v>138</v>
+      </c>
+      <c r="H275">
+        <f>F275/F274 * 100</f>
+        <v>43.830034388180685</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B276">
+        <v>11452224228</v>
+      </c>
+      <c r="C276" t="s">
+        <v>37</v>
+      </c>
+      <c r="F276">
+        <v>12142752553</v>
+      </c>
+      <c r="G276" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B277">
+        <v>5944410</v>
+      </c>
+      <c r="C277" t="s">
+        <v>39</v>
+      </c>
+      <c r="F277">
+        <v>4749891</v>
+      </c>
+      <c r="G277" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B278">
+        <v>12026303336</v>
+      </c>
+      <c r="C278" t="s">
+        <v>139</v>
+      </c>
+      <c r="F278">
+        <v>25759932168</v>
+      </c>
+      <c r="G278" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B279">
+        <v>810</v>
+      </c>
+      <c r="C279" t="s">
+        <v>140</v>
+      </c>
+      <c r="F279">
+        <v>811</v>
+      </c>
+      <c r="G279" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B280">
+        <v>90901.611214999997</v>
+      </c>
+      <c r="C280" t="s">
+        <v>141</v>
+      </c>
+      <c r="F280">
+        <v>194853.09533499999</v>
+      </c>
+      <c r="G280" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B281">
+        <v>90901.639286000005</v>
+      </c>
+      <c r="C281" t="s">
+        <v>12</v>
+      </c>
+      <c r="F281">
+        <v>194853.171397</v>
+      </c>
+      <c r="G281" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B282">
+        <v>173330254152</v>
+      </c>
+      <c r="C282" t="s">
+        <v>23</v>
+      </c>
+      <c r="D282">
+        <f>B282/B272 * 100</f>
+        <v>82.030848007809155</v>
+      </c>
+      <c r="F282">
+        <v>338374680373</v>
+      </c>
+      <c r="G282" t="s">
+        <v>23</v>
+      </c>
+      <c r="H282">
+        <f>F282/F272 * 100</f>
+        <v>89.011109857896429</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B283">
+        <v>122600454269</v>
+      </c>
+      <c r="C283" t="s">
+        <v>27</v>
+      </c>
+      <c r="D283">
+        <f>B283/B272 * 100</f>
+        <v>58.022295524988422</v>
+      </c>
+      <c r="F283">
+        <v>269530286269</v>
+      </c>
+      <c r="G283" t="s">
+        <v>27</v>
+      </c>
+      <c r="H283">
+        <f>F283/F272 * 100</f>
+        <v>70.901256248470077</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>155</v>
+      </c>
+      <c r="B285">
+        <v>376778651800</v>
+      </c>
+      <c r="C285" t="s">
+        <v>20</v>
+      </c>
+      <c r="E285" t="s">
+        <v>156</v>
+      </c>
+      <c r="F285">
+        <v>152496089455</v>
+      </c>
+      <c r="G285" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B286">
+        <v>7473169965</v>
+      </c>
+      <c r="C286" t="s">
+        <v>30</v>
+      </c>
+      <c r="F286">
+        <v>10009113821</v>
+      </c>
+      <c r="G286" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B287">
+        <v>30423843</v>
+      </c>
+      <c r="C287" t="s">
+        <v>137</v>
+      </c>
+      <c r="F287">
+        <v>94211470</v>
+      </c>
+      <c r="G287" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B288">
+        <v>26811664</v>
+      </c>
+      <c r="C288" t="s">
+        <v>138</v>
+      </c>
+      <c r="D288">
+        <f>B288/B287 * 100</f>
+        <v>88.127144226980135</v>
+      </c>
+      <c r="F288">
+        <v>52158138</v>
+      </c>
+      <c r="G288" t="s">
+        <v>138</v>
+      </c>
+      <c r="H288">
+        <f>F288/F287 * 100</f>
+        <v>55.362832147720439</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B289">
+        <v>1344602768</v>
+      </c>
+      <c r="C289" t="s">
+        <v>37</v>
+      </c>
+      <c r="F289">
+        <v>1761602676</v>
+      </c>
+      <c r="G289" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B290">
+        <v>1939706</v>
+      </c>
+      <c r="C290" t="s">
+        <v>39</v>
+      </c>
+      <c r="F290">
+        <v>3789810</v>
+      </c>
+      <c r="G290" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B291">
+        <v>24233635335</v>
+      </c>
+      <c r="C291" t="s">
+        <v>139</v>
+      </c>
+      <c r="F291">
+        <v>8801710751</v>
+      </c>
+      <c r="G291" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B292">
+        <v>811</v>
+      </c>
+      <c r="C292" t="s">
+        <v>140</v>
+      </c>
+      <c r="F292">
+        <v>810</v>
+      </c>
+      <c r="G292" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B293">
+        <v>183676.566529</v>
+      </c>
+      <c r="C293" t="s">
+        <v>141</v>
+      </c>
+      <c r="F293">
+        <v>66581.009468000004</v>
+      </c>
+      <c r="G293" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B294">
+        <v>183677.11167099999</v>
+      </c>
+      <c r="C294" t="s">
+        <v>12</v>
+      </c>
+      <c r="F294">
+        <v>66581.195716999995</v>
+      </c>
+      <c r="G294" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B295">
+        <v>373099076593</v>
+      </c>
+      <c r="C295" t="s">
+        <v>23</v>
+      </c>
+      <c r="D295">
+        <f>B295/B285 * 100</f>
+        <v>99.023411971612134</v>
+      </c>
+      <c r="F295">
+        <v>148261893598</v>
+      </c>
+      <c r="G295" t="s">
+        <v>23</v>
+      </c>
+      <c r="H295">
+        <f>F295/F285 * 100</f>
+        <v>97.223406926608789</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B296">
+        <v>304433278597</v>
+      </c>
+      <c r="C296" t="s">
+        <v>27</v>
+      </c>
+      <c r="D296">
+        <f>B296/B285 * 100</f>
+        <v>80.798972325692688</v>
+      </c>
+      <c r="F296">
+        <v>130977931398</v>
+      </c>
+      <c r="G296" t="s">
+        <v>27</v>
+      </c>
+      <c r="H296">
+        <f>F296/F285 * 100</f>
+        <v>85.889370583925839</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>43</v>
+      </c>
+      <c r="B298">
+        <v>291678068575</v>
+      </c>
+      <c r="C298" t="s">
+        <v>20</v>
+      </c>
+      <c r="E298" t="s">
+        <v>75</v>
+      </c>
+      <c r="F298">
+        <v>26829298828</v>
+      </c>
+      <c r="G298" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B299">
+        <v>27026065319</v>
+      </c>
+      <c r="C299" t="s">
+        <v>30</v>
+      </c>
+      <c r="F299">
+        <v>16724380191</v>
+      </c>
+      <c r="G299" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B300">
+        <v>55899684</v>
+      </c>
+      <c r="C300" t="s">
+        <v>137</v>
+      </c>
+      <c r="F300">
+        <v>20932682</v>
+      </c>
+      <c r="G300" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B301">
+        <v>22463344</v>
+      </c>
+      <c r="C301" t="s">
+        <v>138</v>
+      </c>
+      <c r="D301">
+        <f>B301/B300 * 100</f>
+        <v>40.185100151907839</v>
+      </c>
+      <c r="F301">
+        <v>9259519</v>
+      </c>
+      <c r="G301" t="s">
+        <v>138</v>
+      </c>
+      <c r="H301">
+        <f>F301/F300 * 100</f>
+        <v>44.234747367776379</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B302">
+        <v>9245008504</v>
+      </c>
+      <c r="C302" t="s">
+        <v>37</v>
+      </c>
+      <c r="F302">
+        <v>3954122463</v>
+      </c>
+      <c r="G302" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B303">
+        <v>7583573</v>
+      </c>
+      <c r="C303" t="s">
+        <v>39</v>
+      </c>
+      <c r="F303">
+        <v>5028398</v>
+      </c>
+      <c r="G303" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B304">
+        <v>20689657820</v>
+      </c>
+      <c r="C304" t="s">
+        <v>139</v>
+      </c>
+      <c r="F304">
+        <v>1839664107</v>
+      </c>
+      <c r="G304" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B305">
+        <v>811</v>
+      </c>
+      <c r="C305" t="s">
+        <v>140</v>
+      </c>
+      <c r="F305">
+        <v>810</v>
+      </c>
+      <c r="G305" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B306">
+        <v>156659.36922200001</v>
+      </c>
+      <c r="C306" t="s">
+        <v>141</v>
+      </c>
+      <c r="F306">
+        <v>14292.175730000001</v>
+      </c>
+      <c r="G306" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B307">
+        <v>156660.63276400001</v>
+      </c>
+      <c r="C307" t="s">
+        <v>12</v>
+      </c>
+      <c r="F307">
+        <v>14293.603504000001</v>
+      </c>
+      <c r="G307" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B308">
+        <v>276526511601</v>
+      </c>
+      <c r="C308" t="s">
+        <v>23</v>
+      </c>
+      <c r="D308">
+        <f>B308/B298 * 100</f>
+        <v>94.805383535339743</v>
+      </c>
+      <c r="F308">
+        <v>20147735002</v>
+      </c>
+      <c r="G308" t="s">
+        <v>23</v>
+      </c>
+      <c r="H308">
+        <f>F308/F298 * 100</f>
+        <v>75.096017719900729</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B309">
+        <v>191972396985</v>
+      </c>
+      <c r="C309" t="s">
+        <v>27</v>
+      </c>
+      <c r="D309">
+        <f>B309/B298 * 100</f>
+        <v>65.816534620818629</v>
+      </c>
+      <c r="F309">
+        <v>13465580402</v>
+      </c>
+      <c r="G309" t="s">
+        <v>27</v>
+      </c>
+      <c r="H309">
+        <f>F309/F298 * 100</f>
+        <v>50.189833466489432</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>43</v>
+      </c>
+      <c r="B311">
+        <v>291678068575</v>
+      </c>
+      <c r="C311" t="s">
+        <v>20</v>
+      </c>
+      <c r="E311" t="s">
+        <v>75</v>
+      </c>
+      <c r="F311">
+        <v>26829298828</v>
+      </c>
+      <c r="G311" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B312">
+        <v>27026065319</v>
+      </c>
+      <c r="C312" t="s">
+        <v>30</v>
+      </c>
+      <c r="F312">
+        <v>16724380191</v>
+      </c>
+      <c r="G312" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B313">
+        <v>55899684</v>
+      </c>
+      <c r="C313" t="s">
+        <v>137</v>
+      </c>
+      <c r="F313">
+        <v>20932682</v>
+      </c>
+      <c r="G313" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B314">
+        <v>22463344</v>
+      </c>
+      <c r="C314" t="s">
+        <v>138</v>
+      </c>
+      <c r="D314">
+        <f>B314/B313 * 100</f>
+        <v>40.185100151907839</v>
+      </c>
+      <c r="F314">
+        <v>9259519</v>
+      </c>
+      <c r="G314" t="s">
+        <v>138</v>
+      </c>
+      <c r="H314">
+        <f>F314/F313 * 100</f>
+        <v>44.234747367776379</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B315">
+        <v>9245008504</v>
+      </c>
+      <c r="C315" t="s">
+        <v>37</v>
+      </c>
+      <c r="F315">
+        <v>3954122463</v>
+      </c>
+      <c r="G315" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B316">
+        <v>7583573</v>
+      </c>
+      <c r="C316" t="s">
+        <v>39</v>
+      </c>
+      <c r="F316">
+        <v>5028398</v>
+      </c>
+      <c r="G316" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B317">
+        <v>20689657820</v>
+      </c>
+      <c r="C317" t="s">
+        <v>139</v>
+      </c>
+      <c r="F317">
+        <v>1839664107</v>
+      </c>
+      <c r="G317" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B318">
+        <v>811</v>
+      </c>
+      <c r="C318" t="s">
+        <v>140</v>
+      </c>
+      <c r="F318">
+        <v>810</v>
+      </c>
+      <c r="G318" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B319">
+        <v>156659.36922200001</v>
+      </c>
+      <c r="C319" t="s">
+        <v>141</v>
+      </c>
+      <c r="F319">
+        <v>14292.175730000001</v>
+      </c>
+      <c r="G319" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B320">
+        <v>156660.63276400001</v>
+      </c>
+      <c r="C320" t="s">
+        <v>12</v>
+      </c>
+      <c r="F320">
+        <v>14293.603504000001</v>
+      </c>
+      <c r="G320" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="321" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B321">
+        <v>276526511601</v>
+      </c>
+      <c r="C321" t="s">
+        <v>23</v>
+      </c>
+      <c r="D321">
+        <f>B321/B311 * 100</f>
+        <v>94.805383535339743</v>
+      </c>
+      <c r="F321">
+        <v>20147735002</v>
+      </c>
+      <c r="G321" t="s">
+        <v>23</v>
+      </c>
+      <c r="H321">
+        <f>F321/F311 * 100</f>
+        <v>75.096017719900729</v>
+      </c>
+    </row>
+    <row r="322" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B322">
+        <v>191972396985</v>
+      </c>
+      <c r="C322" t="s">
+        <v>27</v>
+      </c>
+      <c r="D322">
+        <f>B322/B311 * 100</f>
+        <v>65.816534620818629</v>
+      </c>
+      <c r="F322">
+        <v>13465580402</v>
+      </c>
+      <c r="G322" t="s">
+        <v>27</v>
+      </c>
+      <c r="H322">
+        <f>F322/F311 * 100</f>
+        <v>50.189833466489432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in hash table stuff to report
</commit_message>
<xml_diff>
--- a/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
+++ b/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -831,11 +831,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="47532672"/>
-        <c:axId val="48427392"/>
+        <c:axId val="113457408"/>
+        <c:axId val="113594752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47532672"/>
+        <c:axId val="113457408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,7 +864,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48427392"/>
+        <c:crossAx val="113594752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -872,7 +872,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48427392"/>
+        <c:axId val="113594752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="9000000"/>
@@ -903,7 +903,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47532672"/>
+        <c:crossAx val="113457408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1249,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:O256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished converting to present tense, added table numbers
</commit_message>
<xml_diff>
--- a/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
+++ b/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="131">
   <si>
     <t>Stoker Locked</t>
   </si>
@@ -397,6 +397,21 @@
   </si>
   <si>
     <t>Stoker (32 Core) 134217728 CAS lock</t>
+  </si>
+  <si>
+    <t>CASLOCK</t>
+  </si>
+  <si>
+    <t>TASWP</t>
+  </si>
+  <si>
+    <t>Compare-and-swap</t>
+  </si>
+  <si>
+    <t>Test-and-set</t>
+  </si>
+  <si>
+    <t>Test-and-test-and-set</t>
   </si>
 </sst>
 </file>
@@ -460,10 +475,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -904,11 +919,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106547072"/>
-        <c:axId val="106557440"/>
+        <c:axId val="106755968"/>
+        <c:axId val="106504192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106547072"/>
+        <c:axId val="106755968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +952,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106557440"/>
+        <c:crossAx val="106504192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -945,7 +960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106557440"/>
+        <c:axId val="106504192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="9000000"/>
@@ -976,7 +991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106547072"/>
+        <c:crossAx val="106755968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1313,11 +1328,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143467264"/>
-        <c:axId val="143469184"/>
+        <c:axId val="112423680"/>
+        <c:axId val="112425600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143467264"/>
+        <c:axId val="112423680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,7 +1362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143469184"/>
+        <c:crossAx val="112425600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1355,7 +1370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143469184"/>
+        <c:axId val="112425600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1392,7 +1407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143467264"/>
+        <c:crossAx val="112423680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1729,11 +1744,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="158755456"/>
-        <c:axId val="159306496"/>
+        <c:axId val="112476928"/>
+        <c:axId val="112478848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="158755456"/>
+        <c:axId val="112476928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1763,7 +1778,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159306496"/>
+        <c:crossAx val="112478848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1771,7 +1786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159306496"/>
+        <c:axId val="112478848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1823,408 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158755456"/>
+        <c:crossAx val="112476928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Ring Buffer; Stoker; Best Performing Locks; 128</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Key Range</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$W$85</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) CAS lock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$X$84:$AE$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$85:$AE$85</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9341614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7477281</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6762754</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5301549</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6845553</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5428319</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5561829</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5763394</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$W$86</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) TAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$X$84:$AE$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$86:$AE$86</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>9649396</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5527749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5539080</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5575020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7095970</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7173307</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5859077</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7530698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$W$87</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) TTAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$X$84:$AE$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$X$87:$AE$87</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8286680</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8722895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9103403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9121004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7738830</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6135040</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6066340</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6456935</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="119942528"/>
+        <c:axId val="120052736"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="119942528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120052736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="120052736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.5000000000000001E-2"/>
+              <c:y val="0.27795312044327791"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119942528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2035,11 +2451,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="45458944"/>
-        <c:axId val="45460480"/>
+        <c:axId val="106522496"/>
+        <c:axId val="106536960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45458944"/>
+        <c:axId val="106522496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,7 +2485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45460480"/>
+        <c:crossAx val="106536960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2077,7 +2493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45460480"/>
+        <c:axId val="106536960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2114,7 +2530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45458944"/>
+        <c:crossAx val="106522496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2436,11 +2852,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43185280"/>
-        <c:axId val="44636032"/>
+        <c:axId val="106567552"/>
+        <c:axId val="106573824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43185280"/>
+        <c:axId val="106567552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2470,7 +2886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44636032"/>
+        <c:crossAx val="106573824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2478,7 +2894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44636032"/>
+        <c:axId val="106573824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2515,7 +2931,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43185280"/>
+        <c:crossAx val="106567552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2837,11 +3253,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="158494720"/>
-        <c:axId val="158496640"/>
+        <c:axId val="106600320"/>
+        <c:axId val="106602496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="158494720"/>
+        <c:axId val="106600320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2871,7 +3287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158496640"/>
+        <c:crossAx val="106602496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2879,7 +3295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158496640"/>
+        <c:axId val="106602496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,7 +3332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158494720"/>
+        <c:crossAx val="106600320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3164,11 +3580,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="91411968"/>
-        <c:axId val="91419776"/>
+        <c:axId val="106973824"/>
+        <c:axId val="106980096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91411968"/>
+        <c:axId val="106973824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3198,7 +3614,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91419776"/>
+        <c:crossAx val="106980096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3206,7 +3622,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91419776"/>
+        <c:axId val="106980096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3243,7 +3659,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91411968"/>
+        <c:crossAx val="106973824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3573,11 +3989,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="117201536"/>
-        <c:axId val="95826688"/>
+        <c:axId val="106990592"/>
+        <c:axId val="107017344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117201536"/>
+        <c:axId val="106990592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3607,7 +4023,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95826688"/>
+        <c:crossAx val="107017344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3615,7 +4031,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95826688"/>
+        <c:axId val="107017344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3652,7 +4068,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117201536"/>
+        <c:crossAx val="106990592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3974,11 +4390,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="159057408"/>
-        <c:axId val="159059328"/>
+        <c:axId val="107060224"/>
+        <c:axId val="107066496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="159057408"/>
+        <c:axId val="107060224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4008,7 +4424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159059328"/>
+        <c:crossAx val="107066496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4016,7 +4432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159059328"/>
+        <c:axId val="107066496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4053,7 +4469,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159057408"/>
+        <c:crossAx val="107060224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4375,11 +4791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="159845376"/>
-        <c:axId val="159855744"/>
+        <c:axId val="112604288"/>
+        <c:axId val="112606208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="159845376"/>
+        <c:axId val="112604288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4409,7 +4825,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159855744"/>
+        <c:crossAx val="112606208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4417,7 +4833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159855744"/>
+        <c:axId val="112606208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4454,7 +4870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159845376"/>
+        <c:crossAx val="112604288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4799,11 +5215,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="159621888"/>
-        <c:axId val="159623808"/>
+        <c:axId val="112648960"/>
+        <c:axId val="112650880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="159621888"/>
+        <c:axId val="112648960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4833,7 +5249,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159623808"/>
+        <c:crossAx val="112650880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4841,7 +5257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159623808"/>
+        <c:axId val="112650880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4878,7 +5294,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159621888"/>
+        <c:crossAx val="112648960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5250,6 +5666,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5542,8 +5990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:CB256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BT24" sqref="BT24"/>
+    <sheetView tabSelected="1" topLeftCell="R71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X105" sqref="X105:AC108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5563,6 +6011,7 @@
     <col min="19" max="19" width="20.5703125" customWidth="1"/>
     <col min="20" max="20" width="14.28515625" customWidth="1"/>
     <col min="21" max="21" width="12.42578125" customWidth="1"/>
+    <col min="23" max="23" width="25.7109375" customWidth="1"/>
     <col min="24" max="24" width="20.140625" customWidth="1"/>
     <col min="29" max="29" width="29.42578125" customWidth="1"/>
     <col min="30" max="30" width="16.140625" customWidth="1"/>
@@ -5578,17 +6027,17 @@
       <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -8296,17 +8745,17 @@
       <c r="BH50" s="3"/>
     </row>
     <row r="51" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
     </row>
     <row r="52" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B52">
@@ -8391,52 +8840,52 @@
       <c r="N53" t="s">
         <v>91</v>
       </c>
-      <c r="O53" s="9">
+      <c r="O53" s="8">
         <v>79185892878</v>
       </c>
-      <c r="P53" s="9">
+      <c r="P53" s="8">
         <v>13944131</v>
       </c>
-      <c r="Q53" s="9">
+      <c r="Q53" s="8">
         <v>4706821</v>
       </c>
-      <c r="R53" s="9">
+      <c r="R53" s="8">
         <v>54076065449</v>
       </c>
       <c r="AE53" t="s">
         <v>110</v>
       </c>
-      <c r="AF53" s="9">
+      <c r="AF53" s="8">
         <v>89787238122</v>
       </c>
-      <c r="AG53" s="9">
+      <c r="AG53" s="8">
         <v>6509871</v>
       </c>
-      <c r="AH53" s="9">
+      <c r="AH53" s="8">
         <v>1332549</v>
       </c>
-      <c r="AI53" s="9">
+      <c r="AI53" s="8">
         <v>59319590013</v>
       </c>
-      <c r="AJ53" s="9">
+      <c r="AJ53" s="8">
         <v>44995297001</v>
       </c>
       <c r="AV53" t="s">
         <v>116</v>
       </c>
-      <c r="AW53" s="9">
+      <c r="AW53" s="8">
         <v>89787238122</v>
       </c>
-      <c r="AX53" s="9">
+      <c r="AX53" s="8">
         <v>6509871</v>
       </c>
-      <c r="AY53" s="9">
+      <c r="AY53" s="8">
         <v>1332549</v>
       </c>
-      <c r="AZ53" s="9">
+      <c r="AZ53" s="8">
         <v>59319590013</v>
       </c>
-      <c r="BA53" s="9">
+      <c r="BA53" s="8">
         <v>44995297001</v>
       </c>
     </row>
@@ -8455,34 +8904,34 @@
       <c r="N54" t="s">
         <v>92</v>
       </c>
-      <c r="O54" s="9">
+      <c r="O54" s="8">
         <v>2387580464961</v>
       </c>
-      <c r="P54" s="9">
+      <c r="P54" s="8">
         <v>375377904</v>
       </c>
-      <c r="Q54" s="9">
+      <c r="Q54" s="8">
         <v>234272486</v>
       </c>
-      <c r="R54" s="9">
+      <c r="R54" s="8">
         <v>2208662674682</v>
       </c>
       <c r="AE54" t="s">
         <v>111</v>
       </c>
-      <c r="AF54" s="9">
+      <c r="AF54" s="8">
         <v>2658295073696</v>
       </c>
-      <c r="AG54" s="9">
+      <c r="AG54" s="8">
         <v>204921835</v>
       </c>
-      <c r="AH54" s="9">
+      <c r="AH54" s="8">
         <v>183851642</v>
       </c>
-      <c r="AI54" s="9">
+      <c r="AI54" s="8">
         <v>2645119511917</v>
       </c>
-      <c r="AJ54" s="9">
+      <c r="AJ54" s="8">
         <v>2581132930035</v>
       </c>
       <c r="AV54" t="s">
@@ -8519,41 +8968,41 @@
       <c r="N55" t="s">
         <v>105</v>
       </c>
-      <c r="O55" s="9">
+      <c r="O55" s="8">
         <v>2410879761536</v>
       </c>
-      <c r="P55" s="9">
+      <c r="P55" s="8">
         <v>309395431</v>
       </c>
-      <c r="Q55" s="9">
+      <c r="Q55" s="8">
         <v>199455670</v>
       </c>
-      <c r="R55" s="9">
+      <c r="R55" s="8">
         <v>2348280472755</v>
       </c>
       <c r="AE55" t="s">
         <v>112</v>
       </c>
-      <c r="AF55" s="9">
+      <c r="AF55" s="8">
         <v>2666912056805</v>
       </c>
-      <c r="AG55" s="9">
+      <c r="AG55" s="8">
         <v>225390362</v>
       </c>
-      <c r="AH55" s="9">
+      <c r="AH55" s="8">
         <v>207153195</v>
       </c>
-      <c r="AI55" s="9">
+      <c r="AI55" s="8">
         <v>2648994966447</v>
       </c>
-      <c r="AJ55" s="9">
+      <c r="AJ55" s="8">
         <v>2479600299665</v>
       </c>
-      <c r="AW55" s="9"/>
-      <c r="AX55" s="9"/>
-      <c r="AY55" s="9"/>
-      <c r="AZ55" s="9"/>
-      <c r="BA55" s="9"/>
+      <c r="AW55" s="8"/>
+      <c r="AX55" s="8"/>
+      <c r="AY55" s="8"/>
+      <c r="AZ55" s="8"/>
+      <c r="BA55" s="8"/>
     </row>
     <row r="56" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -9132,7 +9581,7 @@
       </c>
       <c r="L80" s="1"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>33</v>
       </c>
@@ -9163,7 +9612,7 @@
       <c r="L81" s="1"/>
       <c r="O81" s="2"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>34</v>
       </c>
@@ -9194,7 +9643,7 @@
       <c r="L82" s="1"/>
       <c r="O82" s="2"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -9224,7 +9673,7 @@
       </c>
       <c r="L83" s="1"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>35</v>
       </c>
@@ -9237,8 +9686,32 @@
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="L84" s="1"/>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="X84">
+        <v>1</v>
+      </c>
+      <c r="Y84">
+        <v>2</v>
+      </c>
+      <c r="Z84">
+        <v>4</v>
+      </c>
+      <c r="AA84">
+        <v>8</v>
+      </c>
+      <c r="AB84">
+        <v>16</v>
+      </c>
+      <c r="AC84">
+        <v>32</v>
+      </c>
+      <c r="AD84">
+        <v>64</v>
+      </c>
+      <c r="AE84">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -9267,8 +9740,35 @@
         <v>774142</v>
       </c>
       <c r="L85" s="1"/>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W85" t="s">
+        <v>42</v>
+      </c>
+      <c r="X85" s="3">
+        <v>9341614</v>
+      </c>
+      <c r="Y85" s="3">
+        <v>7477281</v>
+      </c>
+      <c r="Z85" s="3">
+        <v>6762754</v>
+      </c>
+      <c r="AA85" s="3">
+        <v>5301549</v>
+      </c>
+      <c r="AB85" s="3">
+        <v>6845553</v>
+      </c>
+      <c r="AC85" s="3">
+        <v>5428319</v>
+      </c>
+      <c r="AD85" s="3">
+        <v>5561829</v>
+      </c>
+      <c r="AE85" s="3">
+        <v>5763394</v>
+      </c>
+    </row>
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>15</v>
       </c>
@@ -9298,13 +9798,67 @@
       </c>
       <c r="L86" s="1"/>
       <c r="O86" s="2"/>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W86" t="s">
+        <v>44</v>
+      </c>
+      <c r="X86" s="3">
+        <v>9649396</v>
+      </c>
+      <c r="Y86" s="3">
+        <v>5527749</v>
+      </c>
+      <c r="Z86" s="3">
+        <v>5539080</v>
+      </c>
+      <c r="AA86" s="3">
+        <v>5575020</v>
+      </c>
+      <c r="AB86" s="3">
+        <v>7095970</v>
+      </c>
+      <c r="AC86" s="3">
+        <v>7173307</v>
+      </c>
+      <c r="AD86" s="3">
+        <v>5859077</v>
+      </c>
+      <c r="AE86" s="3">
+        <v>7530698</v>
+      </c>
+    </row>
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="W87" t="s">
+        <v>47</v>
+      </c>
+      <c r="X87" s="3">
+        <v>8286680</v>
+      </c>
+      <c r="Y87" s="3">
+        <v>8722895</v>
+      </c>
+      <c r="Z87" s="3">
+        <v>9103403</v>
+      </c>
+      <c r="AA87" s="3">
+        <v>9121004</v>
+      </c>
+      <c r="AB87" s="3">
+        <v>7738830</v>
+      </c>
+      <c r="AC87" s="3">
+        <v>6135040</v>
+      </c>
+      <c r="AD87" s="3">
+        <v>6066340</v>
+      </c>
+      <c r="AE87" s="3">
+        <v>6456935</v>
+      </c>
+    </row>
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>13</v>
       </c>
@@ -9334,31 +9888,103 @@
       </c>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B91" s="1"/>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B92" s="1"/>
       <c r="E92" s="2"/>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="X92" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y92" s="8">
+        <v>79754534490</v>
+      </c>
+      <c r="Z92" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA92" s="3"/>
+      <c r="AB92" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC92" s="8">
+        <v>85619355140</v>
+      </c>
+      <c r="AD92" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE92" s="3"/>
+      <c r="AF92" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG92" s="8">
+        <v>79316121182</v>
+      </c>
+      <c r="AH92" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI92" s="3"/>
+    </row>
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B93" s="1"/>
       <c r="E93" s="2"/>
       <c r="O93" s="2"/>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y93" s="8">
+        <v>56569249696</v>
+      </c>
+      <c r="Z93" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA93" s="3"/>
+      <c r="AC93" s="8">
+        <v>65574063306</v>
+      </c>
+      <c r="AD93" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE93" s="3"/>
+      <c r="AG93" s="8">
+        <v>59460287672</v>
+      </c>
+      <c r="AH93" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AI93" s="3"/>
+    </row>
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="L94" s="1"/>
       <c r="O94" s="2"/>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y94" s="8">
+        <v>20983294</v>
+      </c>
+      <c r="Z94" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA94" s="3"/>
+      <c r="AC94" s="8">
+        <v>31279956</v>
+      </c>
+      <c r="AD94" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE94" s="3"/>
+      <c r="AG94" s="8">
+        <v>32510859</v>
+      </c>
+      <c r="AH94" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI94" s="3"/>
+    </row>
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>2</v>
       </c>
@@ -9381,15 +10007,66 @@
         <v>128</v>
       </c>
       <c r="L95" s="1"/>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y95" s="8">
+        <v>12112524</v>
+      </c>
+      <c r="Z95" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA95" s="3">
+        <f>Y95/Y94*100</f>
+        <v>57.724607013560401</v>
+      </c>
+      <c r="AC95" s="8">
+        <v>24668363</v>
+      </c>
+      <c r="AD95" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE95" s="3">
+        <f>AC95/AC94*100</f>
+        <v>78.863164001893097</v>
+      </c>
+      <c r="AG95" s="8">
+        <v>25794041</v>
+      </c>
+      <c r="AH95" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI95" s="3">
+        <f>AG95/AG94*100</f>
+        <v>79.339770751674081</v>
+      </c>
+    </row>
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B96" s="4"/>
       <c r="L96" s="1"/>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y96" s="8">
+        <v>11841456725</v>
+      </c>
+      <c r="Z96" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA96" s="3"/>
+      <c r="AC96" s="8">
+        <v>14601368254</v>
+      </c>
+      <c r="AD96" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE96" s="3"/>
+      <c r="AG96" s="8">
+        <v>12673942800</v>
+      </c>
+      <c r="AH96" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI96" s="3"/>
+    </row>
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>78</v>
       </c>
@@ -9416,8 +10093,38 @@
       </c>
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y97" s="8">
+        <v>7309026</v>
+      </c>
+      <c r="Z97" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA97" s="3">
+        <f>Y97/Y96*100</f>
+        <v>6.1724044344721452E-2</v>
+      </c>
+      <c r="AC97" s="8">
+        <v>1785230</v>
+      </c>
+      <c r="AD97" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE97" s="3">
+        <f>AC97/AC96*100</f>
+        <v>1.2226456924753897E-2</v>
+      </c>
+      <c r="AG97" s="8">
+        <v>2038563</v>
+      </c>
+      <c r="AH97" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI97" s="3">
+        <f>AG97/AG96*100</f>
+        <v>1.6084678873570426E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>94</v>
       </c>
@@ -9444,8 +10151,29 @@
       </c>
       <c r="L98" s="1"/>
       <c r="N98" s="2"/>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y98" s="8">
+        <v>7534525334</v>
+      </c>
+      <c r="Z98" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA98" s="3"/>
+      <c r="AC98" s="8">
+        <v>7452509717</v>
+      </c>
+      <c r="AD98" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE98" s="3"/>
+      <c r="AG98" s="8">
+        <v>7451334478</v>
+      </c>
+      <c r="AH98" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI98" s="3"/>
+    </row>
+    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>95</v>
       </c>
@@ -9482,8 +10210,29 @@
       <c r="N99">
         <v>134217728</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y99" s="8">
+        <v>58925.319167000001</v>
+      </c>
+      <c r="Z99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA99" s="3"/>
+      <c r="AC99" s="8">
+        <v>56489.566980000003</v>
+      </c>
+      <c r="AD99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE99" s="3"/>
+      <c r="AG99" s="8">
+        <v>56580.175222999998</v>
+      </c>
+      <c r="AH99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI99" s="3"/>
+    </row>
+    <row r="100" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="K100" t="s">
         <v>104</v>
@@ -9497,8 +10246,29 @@
       <c r="N100" s="4">
         <v>11740401</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y100" s="8">
+        <v>58934.824425999999</v>
+      </c>
+      <c r="Z100" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA100" s="3"/>
+      <c r="AC100" s="8">
+        <v>56489.775742999998</v>
+      </c>
+      <c r="AD100" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE100" s="3"/>
+      <c r="AG100" s="8">
+        <v>56580.397015000002</v>
+      </c>
+      <c r="AH100" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI100" s="3"/>
+    </row>
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>39</v>
       </c>
@@ -9514,8 +10284,38 @@
       <c r="N101" s="4">
         <v>10394564</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y101" s="8">
+        <v>53788668103</v>
+      </c>
+      <c r="Z101" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA101" s="3">
+        <f>Y101/Y92*100</f>
+        <v>67.442771056163934</v>
+      </c>
+      <c r="AC101" s="8">
+        <v>55693698279</v>
+      </c>
+      <c r="AD101" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE101" s="3">
+        <f>AC101/AC92*100</f>
+        <v>65.048023531516634</v>
+      </c>
+      <c r="AG101" s="8">
+        <v>51884855784</v>
+      </c>
+      <c r="AH101" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI101" s="3">
+        <f>AG101/AG92*100</f>
+        <v>65.415271209423125</v>
+      </c>
+    </row>
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>96</v>
       </c>
@@ -9549,8 +10349,38 @@
       <c r="N102" s="3">
         <v>9265828</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Y102" s="8">
+        <v>35033676158</v>
+      </c>
+      <c r="Z102" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA102" s="3">
+        <f>Y102/Y92*100</f>
+        <v>43.926876862898226</v>
+      </c>
+      <c r="AC102" s="8">
+        <v>46920397930</v>
+      </c>
+      <c r="AD102" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE102" s="3">
+        <f>AC102/AC92*100</f>
+        <v>54.801157814466571</v>
+      </c>
+      <c r="AG102" s="8">
+        <v>45500710367</v>
+      </c>
+      <c r="AH102" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI102" s="3">
+        <f>AG102/AG92*100</f>
+        <v>57.366282779503763</v>
+      </c>
+    </row>
+    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>97</v>
       </c>
@@ -9577,7 +10407,7 @@
       </c>
       <c r="K103" s="1"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>98</v>
       </c>
@@ -9604,20 +10434,53 @@
       </c>
       <c r="K104" s="1"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="D105" s="2"/>
       <c r="K105" s="1"/>
-    </row>
-    <row r="106" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="Y105" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z105" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA105" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB105" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC105" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="106" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D106" s="2"/>
       <c r="K106" s="1"/>
       <c r="N106" s="2"/>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="X106" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y106" s="8">
+        <v>85619355140</v>
+      </c>
+      <c r="Z106" s="8">
+        <v>31279956</v>
+      </c>
+      <c r="AA106" s="8">
+        <v>24668363</v>
+      </c>
+      <c r="AB106" s="8">
+        <v>55693698279</v>
+      </c>
+      <c r="AC106" s="8">
+        <v>46920397930</v>
+      </c>
+    </row>
+    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>99</v>
       </c>
@@ -9644,8 +10507,26 @@
       </c>
       <c r="K107" s="1"/>
       <c r="N107" s="2"/>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="X107" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y107" s="8">
+        <v>79316121182</v>
+      </c>
+      <c r="Z107" s="8">
+        <v>32510859</v>
+      </c>
+      <c r="AA107" s="8">
+        <v>25794041</v>
+      </c>
+      <c r="AB107" s="8">
+        <v>51884855784</v>
+      </c>
+      <c r="AC107" s="8">
+        <v>45500710367</v>
+      </c>
+    </row>
+    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>100</v>
       </c>
@@ -9670,8 +10551,26 @@
       <c r="H108" s="4">
         <v>10394564</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="X108" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y108" s="8">
+        <v>79754534490</v>
+      </c>
+      <c r="Z108" s="8">
+        <v>20983294</v>
+      </c>
+      <c r="AA108" s="8">
+        <v>12112524</v>
+      </c>
+      <c r="AB108" s="8">
+        <v>53788668103</v>
+      </c>
+      <c r="AC108" s="8">
+        <v>35033676158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>101</v>
       </c>
@@ -9698,11 +10597,11 @@
       </c>
       <c r="K109" s="1"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="E110" s="2"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O111" s="2"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Redid y axis of graphs to read millions of iterations per second
</commit_message>
<xml_diff>
--- a/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
+++ b/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
@@ -327,9 +327,6 @@
     <t>Cube 134217728</t>
   </si>
   <si>
-    <t>Stoker</t>
-  </si>
-  <si>
     <t>Cube</t>
   </si>
   <si>
@@ -412,14 +409,21 @@
   </si>
   <si>
     <t>Test-and-test-and-set</t>
+  </si>
+  <si>
+    <t>Stoker Lockless</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="#,,\ &quot;M&quot;"/>
+    <numFmt numFmtId="172" formatCode="#.##,,,\ &quot;B&quot;"/>
+    <numFmt numFmtId="173" formatCode="#.##,,\ &quot;M&quot;"/>
+    <numFmt numFmtId="174" formatCode="#.###,,,\ &quot;B&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -464,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -479,6 +483,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -919,11 +927,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106755968"/>
-        <c:axId val="106504192"/>
+        <c:axId val="112064384"/>
+        <c:axId val="111878144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106755968"/>
+        <c:axId val="112064384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -952,7 +960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106504192"/>
+        <c:crossAx val="111878144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -960,7 +968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106504192"/>
+        <c:axId val="111878144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="9000000"/>
@@ -991,7 +999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106755968"/>
+        <c:crossAx val="112064384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1328,11 +1336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112423680"/>
-        <c:axId val="112425600"/>
+        <c:axId val="112292608"/>
+        <c:axId val="112294528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112423680"/>
+        <c:axId val="112292608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1362,7 +1370,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112425600"/>
+        <c:crossAx val="112294528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1370,7 +1378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112425600"/>
+        <c:axId val="112294528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,7 +1396,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1407,9 +1415,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112423680"/>
+        <c:crossAx val="112292608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1744,11 +1755,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112476928"/>
-        <c:axId val="112478848"/>
+        <c:axId val="112345856"/>
+        <c:axId val="112347776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112476928"/>
+        <c:axId val="112345856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,7 +1789,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112478848"/>
+        <c:crossAx val="112347776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1786,7 +1797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112478848"/>
+        <c:axId val="112347776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1804,7 +1815,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1823,9 +1834,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112476928"/>
+        <c:crossAx val="112345856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2145,11 +2159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119942528"/>
-        <c:axId val="120052736"/>
+        <c:axId val="112390912"/>
+        <c:axId val="112392832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119942528"/>
+        <c:axId val="112390912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2179,7 +2193,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120052736"/>
+        <c:crossAx val="112392832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2187,7 +2201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="120052736"/>
+        <c:axId val="112392832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2205,7 +2219,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>IMillions of terations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2214,8 +2228,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.5000000000000001E-2"/>
-              <c:y val="0.27795312044327791"/>
+              <c:x val="1.1458333333333333E-2"/>
+              <c:y val="0.27795320843515248"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2224,9 +2238,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119942528"/>
+        <c:crossAx val="112390912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2271,7 +2288,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Ring Buffer; All Machines; Lockless; All Key Ranges</a:t>
+              <a:t>Ring Buffer; Stoker; Lockless; All Key Ranges</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2290,11 +2307,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$99</c:f>
+              <c:f>Sheet1!$K$100</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Stoker</c:v>
+                  <c:v>Stoker Lockless</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2331,110 +2348,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11740401</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$K$100</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Local</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$L$99:$N$99</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>131072</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>134217728</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$L$101:$N$101</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>10277618</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10713959</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10394564</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$K$101</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Cube</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$L$99:$N$99</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>131072</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>134217728</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$L$102:$N$102</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>11168960</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11539810</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9265828</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2451,11 +2364,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106522496"/>
-        <c:axId val="106536960"/>
+        <c:axId val="111900544"/>
+        <c:axId val="111910912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106522496"/>
+        <c:axId val="111900544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2485,7 +2398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106536960"/>
+        <c:crossAx val="111910912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2493,7 +2406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106536960"/>
+        <c:axId val="111910912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,7 +2424,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>IMillions terations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2530,9 +2443,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106522496"/>
+        <c:crossAx val="111900544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2852,11 +2768,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106567552"/>
-        <c:axId val="106573824"/>
+        <c:axId val="111945600"/>
+        <c:axId val="111947776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106567552"/>
+        <c:axId val="111945600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2886,7 +2802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106573824"/>
+        <c:crossAx val="111947776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2894,7 +2810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106573824"/>
+        <c:axId val="111947776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2912,7 +2828,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>IMillions of terations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2921,8 +2837,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.5000000000000001E-2"/>
-              <c:y val="0.27795312044327791"/>
+              <c:x val="1.4690766746940137E-2"/>
+              <c:y val="0.28082677165354331"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2931,9 +2847,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106567552"/>
+        <c:crossAx val="111945600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3253,11 +3172,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106600320"/>
-        <c:axId val="106602496"/>
+        <c:axId val="111974272"/>
+        <c:axId val="111980544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106600320"/>
+        <c:axId val="111974272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3287,7 +3206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106602496"/>
+        <c:crossAx val="111980544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3295,7 +3214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106602496"/>
+        <c:axId val="111980544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3313,7 +3232,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3322,8 +3241,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.5000000000000001E-2"/>
-              <c:y val="0.27795312044327791"/>
+              <c:x val="1.0601180252036532E-2"/>
+              <c:y val="0.27220608199837087"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3332,9 +3251,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106600320"/>
+        <c:crossAx val="111974272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3580,11 +3502,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106973824"/>
-        <c:axId val="106980096"/>
+        <c:axId val="112481408"/>
+        <c:axId val="112483328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106973824"/>
+        <c:axId val="112481408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3614,7 +3536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106980096"/>
+        <c:crossAx val="112483328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3622,7 +3544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106980096"/>
+        <c:axId val="112483328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3640,7 +3562,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3649,8 +3571,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.5000000000000001E-2"/>
-              <c:y val="0.27795312044327791"/>
+              <c:x val="1.7877492877492879E-2"/>
+              <c:y val="0.2750796452167617"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3659,9 +3581,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106973824"/>
+        <c:crossAx val="112481408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3989,11 +3914,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106990592"/>
-        <c:axId val="107017344"/>
+        <c:axId val="112495616"/>
+        <c:axId val="112522368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106990592"/>
+        <c:axId val="112495616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4023,7 +3948,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107017344"/>
+        <c:crossAx val="112522368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4031,7 +3956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107017344"/>
+        <c:axId val="112522368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4049,7 +3974,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4068,9 +3993,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106990592"/>
+        <c:crossAx val="112495616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4390,11 +4318,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="107060224"/>
-        <c:axId val="107066496"/>
+        <c:axId val="112567808"/>
+        <c:axId val="112569728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107060224"/>
+        <c:axId val="112567808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4424,7 +4352,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107066496"/>
+        <c:crossAx val="112569728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4432,7 +4360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107066496"/>
+        <c:axId val="112569728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4450,7 +4378,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4469,9 +4397,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107060224"/>
+        <c:crossAx val="112567808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4791,11 +4722,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112604288"/>
-        <c:axId val="112606208"/>
+        <c:axId val="112600576"/>
+        <c:axId val="112602496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112604288"/>
+        <c:axId val="112600576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4825,7 +4756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112606208"/>
+        <c:crossAx val="112602496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4833,7 +4764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112606208"/>
+        <c:axId val="112602496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4851,7 +4782,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4870,9 +4801,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112604288"/>
+        <c:crossAx val="112600576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5275,7 +5209,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Iterations per second</a:t>
+                  <a:t>Millions of Iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5297,6 +5231,9 @@
         <c:crossAx val="112648960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -5990,8 +5927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:CB256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X105" sqref="X105:AC108"/>
+    <sheetView tabSelected="1" topLeftCell="BE8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BN33" sqref="BN33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6013,12 +5950,18 @@
     <col min="21" max="21" width="12.42578125" customWidth="1"/>
     <col min="23" max="23" width="25.7109375" customWidth="1"/>
     <col min="24" max="24" width="20.140625" customWidth="1"/>
+    <col min="25" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="29.42578125" customWidth="1"/>
     <col min="30" max="30" width="16.140625" customWidth="1"/>
     <col min="31" max="31" width="18.85546875" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="20.7109375" customWidth="1"/>
     <col min="41" max="41" width="20.85546875" customWidth="1"/>
     <col min="46" max="46" width="26.140625" customWidth="1"/>
+    <col min="49" max="51" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="26.5703125" customWidth="1"/>
     <col min="72" max="72" width="24.140625" customWidth="1"/>
   </cols>
@@ -7135,7 +7078,7 @@
         <v>4820</v>
       </c>
       <c r="BH38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="BI38" s="3">
         <v>10001407</v>
@@ -7280,7 +7223,7 @@
       <c r="BB39" s="3"/>
       <c r="BC39" s="3"/>
       <c r="BH39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BI39">
         <v>10004191</v>
@@ -7383,7 +7326,7 @@
       </c>
       <c r="U40" s="3"/>
       <c r="W40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X40" s="3">
         <v>2410879761536</v>
@@ -7393,7 +7336,7 @@
       </c>
       <c r="Z40" s="3"/>
       <c r="AD40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AE40" s="3">
         <v>89787238122</v>
@@ -7403,7 +7346,7 @@
       </c>
       <c r="AG40" s="3"/>
       <c r="AI40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ40" s="3">
         <v>2658295073696</v>
@@ -7413,7 +7356,7 @@
       </c>
       <c r="AL40" s="3"/>
       <c r="AN40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AO40" s="3">
         <v>2666912056805</v>
@@ -7423,7 +7366,7 @@
       </c>
       <c r="AQ40" s="3"/>
       <c r="AU40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AV40" s="3">
         <v>83535405810</v>
@@ -7433,7 +7376,7 @@
       </c>
       <c r="AX40" s="3"/>
       <c r="AZ40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BA40" s="3">
         <v>2934049791690</v>
@@ -7445,7 +7388,7 @@
       <c r="BF40" s="3"/>
       <c r="BG40" s="3"/>
       <c r="BH40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="BI40">
         <v>9700337</v>
@@ -7586,7 +7529,7 @@
       <c r="BF41" s="3"/>
       <c r="BG41" s="3"/>
       <c r="BH41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="BI41" s="3">
         <v>9884624</v>
@@ -7727,7 +7670,7 @@
       <c r="BF42" s="3"/>
       <c r="BG42" s="3"/>
       <c r="BH42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="BI42">
         <v>9872272</v>
@@ -7892,7 +7835,7 @@
       <c r="BF43" s="3"/>
       <c r="BG43" s="3"/>
       <c r="BH43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BI43">
         <v>9495736</v>
@@ -8033,7 +7976,7 @@
       <c r="BF44" s="3"/>
       <c r="BG44" s="3"/>
       <c r="BH44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="BI44" s="3">
         <v>9761450</v>
@@ -8198,7 +8141,7 @@
       <c r="BF45" s="3"/>
       <c r="BG45" s="3"/>
       <c r="BH45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BI45">
         <v>9742855</v>
@@ -8339,7 +8282,7 @@
       <c r="BF46" s="3"/>
       <c r="BG46" s="3"/>
       <c r="BH46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="BI46">
         <v>9341134</v>
@@ -8783,46 +8726,46 @@
         <v>128</v>
       </c>
       <c r="O52" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="P52" t="s">
         <v>106</v>
       </c>
-      <c r="P52" t="s">
+      <c r="Q52" t="s">
         <v>107</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="R52" t="s">
         <v>108</v>
       </c>
-      <c r="R52" t="s">
-        <v>109</v>
-      </c>
       <c r="AF52" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AG52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AH52" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI52" t="s">
         <v>108</v>
       </c>
-      <c r="AI52" t="s">
-        <v>109</v>
-      </c>
       <c r="AJ52" t="s">
+        <v>112</v>
+      </c>
+      <c r="AW52" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX52" t="s">
         <v>113</v>
       </c>
-      <c r="AW52" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AX52" t="s">
-        <v>114</v>
-      </c>
       <c r="AY52" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ52" t="s">
         <v>108</v>
       </c>
-      <c r="AZ52" t="s">
-        <v>109</v>
-      </c>
       <c r="BA52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:60" x14ac:dyDescent="0.25">
@@ -8840,52 +8783,52 @@
       <c r="N53" t="s">
         <v>91</v>
       </c>
-      <c r="O53" s="8">
+      <c r="O53" s="13">
         <v>79185892878</v>
       </c>
-      <c r="P53" s="8">
+      <c r="P53" s="12">
         <v>13944131</v>
       </c>
-      <c r="Q53" s="8">
+      <c r="Q53" s="12">
         <v>4706821</v>
       </c>
-      <c r="R53" s="8">
+      <c r="R53" s="13">
         <v>54076065449</v>
       </c>
       <c r="AE53" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF53" s="8">
+        <v>109</v>
+      </c>
+      <c r="AF53" s="13">
         <v>89787238122</v>
       </c>
-      <c r="AG53" s="8">
+      <c r="AG53" s="12">
         <v>6509871</v>
       </c>
-      <c r="AH53" s="8">
+      <c r="AH53" s="12">
         <v>1332549</v>
       </c>
-      <c r="AI53" s="8">
+      <c r="AI53" s="13">
         <v>59319590013</v>
       </c>
-      <c r="AJ53" s="8">
+      <c r="AJ53" s="13">
         <v>44995297001</v>
       </c>
       <c r="AV53" t="s">
-        <v>116</v>
-      </c>
-      <c r="AW53" s="8">
+        <v>115</v>
+      </c>
+      <c r="AW53" s="13">
         <v>89787238122</v>
       </c>
-      <c r="AX53" s="8">
+      <c r="AX53" s="12">
         <v>6509871</v>
       </c>
-      <c r="AY53" s="8">
+      <c r="AY53" s="12">
         <v>1332549</v>
       </c>
-      <c r="AZ53" s="8">
+      <c r="AZ53" s="13">
         <v>59319590013</v>
       </c>
-      <c r="BA53" s="8">
+      <c r="BA53" s="13">
         <v>44995297001</v>
       </c>
     </row>
@@ -8904,52 +8847,52 @@
       <c r="N54" t="s">
         <v>92</v>
       </c>
-      <c r="O54" s="8">
+      <c r="O54" s="13">
         <v>2387580464961</v>
       </c>
-      <c r="P54" s="8">
+      <c r="P54" s="12">
         <v>375377904</v>
       </c>
-      <c r="Q54" s="8">
+      <c r="Q54" s="12">
         <v>234272486</v>
       </c>
-      <c r="R54" s="8">
+      <c r="R54" s="13">
         <v>2208662674682</v>
       </c>
       <c r="AE54" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF54" s="8">
+        <v>110</v>
+      </c>
+      <c r="AF54" s="13">
         <v>2658295073696</v>
       </c>
-      <c r="AG54" s="8">
+      <c r="AG54" s="12">
         <v>204921835</v>
       </c>
-      <c r="AH54" s="8">
+      <c r="AH54" s="12">
         <v>183851642</v>
       </c>
-      <c r="AI54" s="8">
+      <c r="AI54" s="13">
         <v>2645119511917</v>
       </c>
-      <c r="AJ54" s="8">
+      <c r="AJ54" s="13">
         <v>2581132930035</v>
       </c>
       <c r="AV54" t="s">
-        <v>115</v>
-      </c>
-      <c r="AW54" s="3">
+        <v>114</v>
+      </c>
+      <c r="AW54" s="13">
         <v>2934049791690</v>
       </c>
-      <c r="AX54" s="3">
+      <c r="AX54" s="12">
         <v>398996096</v>
       </c>
-      <c r="AY54" s="3">
+      <c r="AY54" s="12">
         <v>218057504</v>
       </c>
-      <c r="AZ54" s="3">
+      <c r="AZ54" s="13">
         <v>2681775597817</v>
       </c>
-      <c r="BA54" s="3">
+      <c r="BA54" s="13">
         <v>2282696119508</v>
       </c>
     </row>
@@ -8966,36 +8909,36 @@
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="N55" t="s">
-        <v>105</v>
-      </c>
-      <c r="O55" s="8">
+        <v>104</v>
+      </c>
+      <c r="O55" s="13">
         <v>2410879761536</v>
       </c>
-      <c r="P55" s="8">
+      <c r="P55" s="12">
         <v>309395431</v>
       </c>
-      <c r="Q55" s="8">
+      <c r="Q55" s="12">
         <v>199455670</v>
       </c>
-      <c r="R55" s="8">
+      <c r="R55" s="13">
         <v>2348280472755</v>
       </c>
       <c r="AE55" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF55" s="8">
+        <v>111</v>
+      </c>
+      <c r="AF55" s="13">
         <v>2666912056805</v>
       </c>
-      <c r="AG55" s="8">
+      <c r="AG55" s="12">
         <v>225390362</v>
       </c>
-      <c r="AH55" s="8">
+      <c r="AH55" s="12">
         <v>207153195</v>
       </c>
-      <c r="AI55" s="8">
+      <c r="AI55" s="13">
         <v>2648994966447</v>
       </c>
-      <c r="AJ55" s="8">
+      <c r="AJ55" s="13">
         <v>2479600299665</v>
       </c>
       <c r="AW55" s="8"/>
@@ -9912,7 +9855,7 @@
       </c>
       <c r="AA92" s="3"/>
       <c r="AB92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC92" s="8">
         <v>85619355140</v>
@@ -9922,7 +9865,7 @@
       </c>
       <c r="AE92" s="3"/>
       <c r="AF92" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AG92" s="8">
         <v>79316121182</v>
@@ -10198,9 +10141,6 @@
       <c r="H99" s="4">
         <v>11168960</v>
       </c>
-      <c r="K99" t="s">
-        <v>102</v>
-      </c>
       <c r="L99">
         <v>128</v>
       </c>
@@ -10235,7 +10175,7 @@
     <row r="100" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="K100" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="L100" s="4">
         <v>12433048</v>
@@ -10272,7 +10212,7 @@
       <c r="A101" t="s">
         <v>39</v>
       </c>
-      <c r="K101" s="1" t="s">
+      <c r="K101" t="s">
         <v>103</v>
       </c>
       <c r="L101" s="4">
@@ -10339,6 +10279,9 @@
       </c>
       <c r="H102" s="4">
         <v>9419968</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="L102" s="4">
         <v>11168960</v>
@@ -10439,19 +10382,19 @@
       <c r="D105" s="2"/>
       <c r="K105" s="1"/>
       <c r="Y105" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Z105" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AA105" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB105" t="s">
         <v>108</v>
       </c>
-      <c r="AB105" t="s">
-        <v>109</v>
-      </c>
       <c r="AC105" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:35" ht="30" x14ac:dyDescent="0.25">
@@ -10462,21 +10405,21 @@
       <c r="K106" s="1"/>
       <c r="N106" s="2"/>
       <c r="X106" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y106" s="8">
+        <v>127</v>
+      </c>
+      <c r="Y106" s="11">
         <v>85619355140</v>
       </c>
-      <c r="Z106" s="8">
+      <c r="Z106" s="12">
         <v>31279956</v>
       </c>
-      <c r="AA106" s="8">
+      <c r="AA106" s="12">
         <v>24668363</v>
       </c>
-      <c r="AB106" s="8">
+      <c r="AB106" s="11">
         <v>55693698279</v>
       </c>
-      <c r="AC106" s="8">
+      <c r="AC106" s="11">
         <v>46920397930</v>
       </c>
     </row>
@@ -10508,21 +10451,21 @@
       <c r="K107" s="1"/>
       <c r="N107" s="2"/>
       <c r="X107" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y107" s="8">
+        <v>128</v>
+      </c>
+      <c r="Y107" s="11">
         <v>79316121182</v>
       </c>
-      <c r="Z107" s="8">
+      <c r="Z107" s="12">
         <v>32510859</v>
       </c>
-      <c r="AA107" s="8">
+      <c r="AA107" s="12">
         <v>25794041</v>
       </c>
-      <c r="AB107" s="8">
+      <c r="AB107" s="11">
         <v>51884855784</v>
       </c>
-      <c r="AC107" s="8">
+      <c r="AC107" s="11">
         <v>45500710367</v>
       </c>
     </row>
@@ -10552,21 +10495,21 @@
         <v>10394564</v>
       </c>
       <c r="X108" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y108" s="8">
+        <v>129</v>
+      </c>
+      <c r="Y108" s="11">
         <v>79754534490</v>
       </c>
-      <c r="Z108" s="8">
+      <c r="Z108" s="12">
         <v>20983294</v>
       </c>
-      <c r="AA108" s="8">
+      <c r="AA108" s="12">
         <v>12112524</v>
       </c>
-      <c r="AB108" s="8">
+      <c r="AB108" s="11">
         <v>53788668103</v>
       </c>
-      <c r="AC108" s="8">
+      <c r="AC108" s="11">
         <v>35033676158</v>
       </c>
     </row>
@@ -10600,6 +10543,7 @@
     <row r="110" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="E110" s="2"/>
+      <c r="Y110" s="10"/>
     </row>
     <row r="111" spans="1:35" x14ac:dyDescent="0.25">
       <c r="O111" s="2"/>

</xml_diff>

<commit_message>
Went through ring buffer evaluation again, got it up to scratch
</commit_message>
<xml_diff>
--- a/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
+++ b/Data Structures/Ring_Buffer/Ring_Buffer_Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="131">
   <si>
     <t>Stoker Locked</t>
   </si>
@@ -420,10 +420,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="#,,\ &quot;M&quot;"/>
-    <numFmt numFmtId="172" formatCode="#.##,,,\ &quot;B&quot;"/>
-    <numFmt numFmtId="173" formatCode="#.##,,\ &quot;M&quot;"/>
-    <numFmt numFmtId="174" formatCode="#.###,,,\ &quot;B&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,,\ &quot;M&quot;"/>
+    <numFmt numFmtId="165" formatCode="#.##,,,\ &quot;B&quot;"/>
+    <numFmt numFmtId="166" formatCode="#.##,,\ &quot;M&quot;"/>
+    <numFmt numFmtId="167" formatCode="#.###,,,\ &quot;B&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -480,13 +480,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -927,11 +927,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112064384"/>
-        <c:axId val="111878144"/>
+        <c:axId val="101582720"/>
+        <c:axId val="101593088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112064384"/>
+        <c:axId val="101582720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111878144"/>
+        <c:crossAx val="101593088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -968,7 +968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111878144"/>
+        <c:axId val="101593088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="9000000"/>
@@ -999,7 +999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112064384"/>
+        <c:crossAx val="101582720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1336,11 +1336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112292608"/>
-        <c:axId val="112294528"/>
+        <c:axId val="102742272"/>
+        <c:axId val="102756736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112292608"/>
+        <c:axId val="102742272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1370,7 +1370,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112294528"/>
+        <c:crossAx val="102756736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1378,7 +1378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112294528"/>
+        <c:axId val="102756736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1415,7 +1415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112292608"/>
+        <c:crossAx val="102742272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -1755,11 +1755,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112345856"/>
-        <c:axId val="112347776"/>
+        <c:axId val="102402688"/>
+        <c:axId val="102413056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112345856"/>
+        <c:axId val="102402688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,7 +1789,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112347776"/>
+        <c:crossAx val="102413056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1797,7 +1797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112347776"/>
+        <c:axId val="102413056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,7 +1834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112345856"/>
+        <c:crossAx val="102402688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2159,11 +2159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112390912"/>
-        <c:axId val="112392832"/>
+        <c:axId val="102505472"/>
+        <c:axId val="102519936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112390912"/>
+        <c:axId val="102505472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2193,7 +2193,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112392832"/>
+        <c:crossAx val="102519936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2201,7 +2201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112392832"/>
+        <c:axId val="102519936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2238,7 +2238,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112390912"/>
+        <c:crossAx val="102505472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2341,13 +2341,13 @@
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12433048</c:v>
+                  <c:v>10931178</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9419968</c:v>
+                  <c:v>9816335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11740401</c:v>
+                  <c:v>12247141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2364,11 +2364,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111900544"/>
-        <c:axId val="111910912"/>
+        <c:axId val="101613952"/>
+        <c:axId val="101615872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111900544"/>
+        <c:axId val="101613952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2398,7 +2398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111910912"/>
+        <c:crossAx val="101615872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2406,7 +2406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111910912"/>
+        <c:axId val="101615872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2424,7 +2424,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>IMillions terations per second</a:t>
+                  <a:t>Millions of iterations per second</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2443,7 +2443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111900544"/>
+        <c:crossAx val="101613952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -2768,11 +2768,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111945600"/>
-        <c:axId val="111947776"/>
+        <c:axId val="101651200"/>
+        <c:axId val="101653120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111945600"/>
+        <c:axId val="101651200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2802,7 +2802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111947776"/>
+        <c:crossAx val="101653120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2810,7 +2810,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111947776"/>
+        <c:axId val="101653120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2847,7 +2847,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111945600"/>
+        <c:crossAx val="101651200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -3172,11 +3172,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="111974272"/>
-        <c:axId val="111980544"/>
+        <c:axId val="101684352"/>
+        <c:axId val="101686272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="111974272"/>
+        <c:axId val="101684352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3206,7 +3206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111980544"/>
+        <c:crossAx val="101686272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3214,7 +3214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="111980544"/>
+        <c:axId val="101686272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3251,7 +3251,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111974272"/>
+        <c:crossAx val="101684352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -3502,11 +3502,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112481408"/>
-        <c:axId val="112483328"/>
+        <c:axId val="102586624"/>
+        <c:axId val="102592896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112481408"/>
+        <c:axId val="102586624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,7 +3536,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112483328"/>
+        <c:crossAx val="102592896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3544,7 +3544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112483328"/>
+        <c:axId val="102592896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3581,7 +3581,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112481408"/>
+        <c:crossAx val="102586624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -3914,11 +3914,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112495616"/>
-        <c:axId val="112522368"/>
+        <c:axId val="102611584"/>
+        <c:axId val="102634240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112495616"/>
+        <c:axId val="102611584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3948,7 +3948,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112522368"/>
+        <c:crossAx val="102634240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3956,7 +3956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112522368"/>
+        <c:axId val="102634240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3993,7 +3993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112495616"/>
+        <c:crossAx val="102611584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4318,11 +4318,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112567808"/>
-        <c:axId val="112569728"/>
+        <c:axId val="102667776"/>
+        <c:axId val="102669696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112567808"/>
+        <c:axId val="102667776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4352,7 +4352,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112569728"/>
+        <c:crossAx val="102669696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4360,7 +4360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112569728"/>
+        <c:axId val="102669696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4397,7 +4397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112567808"/>
+        <c:crossAx val="102667776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -4722,11 +4722,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112600576"/>
-        <c:axId val="112602496"/>
+        <c:axId val="102778752"/>
+        <c:axId val="102785024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112600576"/>
+        <c:axId val="102778752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4756,7 +4756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112602496"/>
+        <c:crossAx val="102785024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4764,7 +4764,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112602496"/>
+        <c:axId val="102785024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4801,7 +4801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112600576"/>
+        <c:crossAx val="102778752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -5149,11 +5149,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112648960"/>
-        <c:axId val="112650880"/>
+        <c:axId val="102700928"/>
+        <c:axId val="102707200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112648960"/>
+        <c:axId val="102700928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5183,7 +5183,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112650880"/>
+        <c:crossAx val="102707200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5191,7 +5191,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="112650880"/>
+        <c:axId val="102707200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5228,7 +5228,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112648960"/>
+        <c:crossAx val="102700928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
@@ -5287,16 +5287,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>242887</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5927,8 +5927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:CB256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BN33" sqref="BN33"/>
+    <sheetView tabSelected="1" topLeftCell="AL22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M122" sqref="M122:R125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5970,17 +5970,17 @@
       <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -8688,17 +8688,17 @@
       <c r="BH50" s="3"/>
     </row>
     <row r="51" spans="1:60" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
     </row>
     <row r="52" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B52">
@@ -8783,52 +8783,52 @@
       <c r="N53" t="s">
         <v>91</v>
       </c>
-      <c r="O53" s="13">
+      <c r="O53" s="12">
         <v>79185892878</v>
       </c>
-      <c r="P53" s="12">
+      <c r="P53" s="11">
         <v>13944131</v>
       </c>
-      <c r="Q53" s="12">
+      <c r="Q53" s="11">
         <v>4706821</v>
       </c>
-      <c r="R53" s="13">
+      <c r="R53" s="12">
         <v>54076065449</v>
       </c>
       <c r="AE53" t="s">
         <v>109</v>
       </c>
-      <c r="AF53" s="13">
+      <c r="AF53" s="12">
         <v>89787238122</v>
       </c>
-      <c r="AG53" s="12">
+      <c r="AG53" s="11">
         <v>6509871</v>
       </c>
-      <c r="AH53" s="12">
+      <c r="AH53" s="11">
         <v>1332549</v>
       </c>
-      <c r="AI53" s="13">
+      <c r="AI53" s="12">
         <v>59319590013</v>
       </c>
-      <c r="AJ53" s="13">
+      <c r="AJ53" s="12">
         <v>44995297001</v>
       </c>
       <c r="AV53" t="s">
         <v>115</v>
       </c>
-      <c r="AW53" s="13">
+      <c r="AW53" s="12">
         <v>89787238122</v>
       </c>
-      <c r="AX53" s="12">
+      <c r="AX53" s="11">
         <v>6509871</v>
       </c>
-      <c r="AY53" s="12">
+      <c r="AY53" s="11">
         <v>1332549</v>
       </c>
-      <c r="AZ53" s="13">
+      <c r="AZ53" s="12">
         <v>59319590013</v>
       </c>
-      <c r="BA53" s="13">
+      <c r="BA53" s="12">
         <v>44995297001</v>
       </c>
     </row>
@@ -8847,52 +8847,52 @@
       <c r="N54" t="s">
         <v>92</v>
       </c>
-      <c r="O54" s="13">
+      <c r="O54" s="12">
         <v>2387580464961</v>
       </c>
-      <c r="P54" s="12">
+      <c r="P54" s="11">
         <v>375377904</v>
       </c>
-      <c r="Q54" s="12">
+      <c r="Q54" s="11">
         <v>234272486</v>
       </c>
-      <c r="R54" s="13">
+      <c r="R54" s="12">
         <v>2208662674682</v>
       </c>
       <c r="AE54" t="s">
         <v>110</v>
       </c>
-      <c r="AF54" s="13">
+      <c r="AF54" s="12">
         <v>2658295073696</v>
       </c>
-      <c r="AG54" s="12">
+      <c r="AG54" s="11">
         <v>204921835</v>
       </c>
-      <c r="AH54" s="12">
+      <c r="AH54" s="11">
         <v>183851642</v>
       </c>
-      <c r="AI54" s="13">
+      <c r="AI54" s="12">
         <v>2645119511917</v>
       </c>
-      <c r="AJ54" s="13">
+      <c r="AJ54" s="12">
         <v>2581132930035</v>
       </c>
       <c r="AV54" t="s">
         <v>114</v>
       </c>
-      <c r="AW54" s="13">
+      <c r="AW54" s="12">
         <v>2934049791690</v>
       </c>
-      <c r="AX54" s="12">
+      <c r="AX54" s="11">
         <v>398996096</v>
       </c>
-      <c r="AY54" s="12">
+      <c r="AY54" s="11">
         <v>218057504</v>
       </c>
-      <c r="AZ54" s="13">
+      <c r="AZ54" s="12">
         <v>2681775597817</v>
       </c>
-      <c r="BA54" s="13">
+      <c r="BA54" s="12">
         <v>2282696119508</v>
       </c>
     </row>
@@ -8911,34 +8911,34 @@
       <c r="N55" t="s">
         <v>104</v>
       </c>
-      <c r="O55" s="13">
+      <c r="O55" s="12">
         <v>2410879761536</v>
       </c>
-      <c r="P55" s="12">
+      <c r="P55" s="11">
         <v>309395431</v>
       </c>
-      <c r="Q55" s="12">
+      <c r="Q55" s="11">
         <v>199455670</v>
       </c>
-      <c r="R55" s="13">
+      <c r="R55" s="12">
         <v>2348280472755</v>
       </c>
       <c r="AE55" t="s">
         <v>111</v>
       </c>
-      <c r="AF55" s="13">
+      <c r="AF55" s="12">
         <v>2666912056805</v>
       </c>
-      <c r="AG55" s="12">
+      <c r="AG55" s="11">
         <v>225390362</v>
       </c>
-      <c r="AH55" s="12">
+      <c r="AH55" s="11">
         <v>207153195</v>
       </c>
-      <c r="AI55" s="13">
+      <c r="AI55" s="12">
         <v>2648994966447</v>
       </c>
-      <c r="AJ55" s="13">
+      <c r="AJ55" s="12">
         <v>2479600299665</v>
       </c>
       <c r="AW55" s="8"/>
@@ -10178,13 +10178,13 @@
         <v>130</v>
       </c>
       <c r="L100" s="4">
-        <v>12433048</v>
+        <v>10931178</v>
       </c>
       <c r="M100" s="4">
-        <v>9419968</v>
+        <v>9816335</v>
       </c>
       <c r="N100" s="4">
-        <v>11740401</v>
+        <v>12247141</v>
       </c>
       <c r="Y100" s="8">
         <v>58934.824425999999</v>
@@ -10407,19 +10407,19 @@
       <c r="X106" t="s">
         <v>127</v>
       </c>
-      <c r="Y106" s="11">
+      <c r="Y106" s="10">
         <v>85619355140</v>
       </c>
-      <c r="Z106" s="12">
+      <c r="Z106" s="11">
         <v>31279956</v>
       </c>
-      <c r="AA106" s="12">
+      <c r="AA106" s="11">
         <v>24668363</v>
       </c>
-      <c r="AB106" s="11">
+      <c r="AB106" s="10">
         <v>55693698279</v>
       </c>
-      <c r="AC106" s="11">
+      <c r="AC106" s="10">
         <v>46920397930</v>
       </c>
     </row>
@@ -10453,19 +10453,19 @@
       <c r="X107" t="s">
         <v>128</v>
       </c>
-      <c r="Y107" s="11">
+      <c r="Y107" s="10">
         <v>79316121182</v>
       </c>
-      <c r="Z107" s="12">
+      <c r="Z107" s="11">
         <v>32510859</v>
       </c>
-      <c r="AA107" s="12">
+      <c r="AA107" s="11">
         <v>25794041</v>
       </c>
-      <c r="AB107" s="11">
+      <c r="AB107" s="10">
         <v>51884855784</v>
       </c>
-      <c r="AC107" s="11">
+      <c r="AC107" s="10">
         <v>45500710367</v>
       </c>
     </row>
@@ -10497,19 +10497,19 @@
       <c r="X108" t="s">
         <v>129</v>
       </c>
-      <c r="Y108" s="11">
+      <c r="Y108" s="10">
         <v>79754534490</v>
       </c>
-      <c r="Z108" s="12">
+      <c r="Z108" s="11">
         <v>20983294</v>
       </c>
-      <c r="AA108" s="12">
+      <c r="AA108" s="11">
         <v>12112524</v>
       </c>
-      <c r="AB108" s="11">
+      <c r="AB108" s="10">
         <v>53788668103</v>
       </c>
-      <c r="AC108" s="11">
+      <c r="AC108" s="10">
         <v>35033676158</v>
       </c>
     </row>
@@ -10543,27 +10543,226 @@
     <row r="110" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B110" s="1"/>
       <c r="E110" s="2"/>
-      <c r="Y110" s="10"/>
+      <c r="L110">
+        <v>128</v>
+      </c>
+      <c r="M110" s="12">
+        <v>15231440651</v>
+      </c>
+      <c r="N110" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O110" s="3"/>
+      <c r="P110">
+        <v>131072</v>
+      </c>
+      <c r="Q110" s="12">
+        <v>16009556986</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="S110" s="3"/>
+      <c r="T110">
+        <v>134217728</v>
+      </c>
+      <c r="U110" s="12">
+        <v>18566267830</v>
+      </c>
+      <c r="V110" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="W110" s="3"/>
+      <c r="Y110" s="9"/>
     </row>
     <row r="111" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="O111" s="2"/>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M111" s="12">
+        <v>11626660635</v>
+      </c>
+      <c r="N111" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="O111" s="3"/>
+      <c r="Q111" s="12">
+        <v>11862206209</v>
+      </c>
+      <c r="R111" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="S111" s="3"/>
+      <c r="U111" s="12">
+        <v>9148016072</v>
+      </c>
+      <c r="V111" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="W111" s="3"/>
+    </row>
+    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="M112" s="11">
+        <v>4270922</v>
+      </c>
+      <c r="N112" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O112" s="3"/>
+      <c r="Q112" s="11">
+        <v>8838189</v>
+      </c>
+      <c r="R112" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="S112" s="3"/>
+      <c r="U112" s="11">
+        <v>18145926</v>
+      </c>
+      <c r="V112" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="W112" s="3"/>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M113" s="11">
+        <v>3845831</v>
+      </c>
+      <c r="N113" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="O113" s="3">
+        <f>M113/M112*100</f>
+        <v>90.046856393069234</v>
+      </c>
+      <c r="Q113" s="11">
+        <v>8243551</v>
+      </c>
+      <c r="R113" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S113" s="3">
+        <f>Q113/Q112*100</f>
+        <v>93.271947454393654</v>
+      </c>
+      <c r="U113" s="11">
+        <v>17122446</v>
+      </c>
+      <c r="V113" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="W113" s="3">
+        <f>U113/U112*100</f>
+        <v>94.359725703719945</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>77</v>
       </c>
-      <c r="L114" s="1"/>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M114" s="12">
+        <v>2327823906</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O114" s="3"/>
+      <c r="Q114" s="12">
+        <v>2520570838</v>
+      </c>
+      <c r="R114" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S114" s="3"/>
+      <c r="U114" s="12">
+        <v>1716006441</v>
+      </c>
+      <c r="V114" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W114" s="3"/>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M115" s="11">
+        <v>180583</v>
+      </c>
+      <c r="N115" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O115" s="3">
+        <f>M115/M114*100</f>
+        <v>7.7575885158041678E-3</v>
+      </c>
+      <c r="Q115" s="11">
+        <v>282661</v>
+      </c>
+      <c r="R115" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="S115" s="3">
+        <f>Q115/Q114*100</f>
+        <v>1.1214166082484843E-2</v>
+      </c>
+      <c r="U115" s="11">
+        <v>597778</v>
+      </c>
+      <c r="V115" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="W115" s="3">
+        <f>U115/U114*100</f>
+        <v>3.4835417030931765E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>78</v>
       </c>
       <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M116" s="12">
+        <v>991248930</v>
+      </c>
+      <c r="N116" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="O116" s="3"/>
+      <c r="Q116" s="12">
+        <v>1063554668</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S116" s="3"/>
+      <c r="U116" s="12">
+        <v>1222139681</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="W116" s="3"/>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M117" s="11">
+        <v>7514.0927789999996</v>
+      </c>
+      <c r="N117" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="O117" s="3"/>
+      <c r="Q117" s="11">
+        <v>8062.7323930000002</v>
+      </c>
+      <c r="R117" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S117" s="3"/>
+      <c r="U117" s="11">
+        <v>9247.2739089999995</v>
+      </c>
+      <c r="V117" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="W117" s="3"/>
+    </row>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>79</v>
       </c>
@@ -10575,8 +10774,29 @@
       </c>
       <c r="D118" s="3"/>
       <c r="E118" s="2"/>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M118" s="11">
+        <v>7514.0971229999996</v>
+      </c>
+      <c r="N118" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="O118" s="3"/>
+      <c r="Q118" s="11">
+        <v>8062.7421510000004</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="S118" s="3"/>
+      <c r="U118" s="11">
+        <v>9247.2773739999993</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="W118" s="3"/>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B119" s="3">
         <v>184556681008</v>
       </c>
@@ -10585,9 +10805,38 @@
       </c>
       <c r="D119" s="3"/>
       <c r="E119" s="2"/>
-      <c r="O119" s="2"/>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M119" s="12">
+        <v>10140918426</v>
+      </c>
+      <c r="N119" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="O119" s="3">
+        <f>M119/M110*100</f>
+        <v>66.578852640142159</v>
+      </c>
+      <c r="Q119" s="12">
+        <v>10574451072</v>
+      </c>
+      <c r="R119" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="S119" s="3">
+        <f>Q119/Q110*100</f>
+        <v>66.050866249747713</v>
+      </c>
+      <c r="U119" s="12">
+        <v>14199910081</v>
+      </c>
+      <c r="V119" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="W119" s="3">
+        <f>U119/U110*100</f>
+        <v>76.482307650734782</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B120" s="3">
         <v>452061027</v>
       </c>
@@ -10595,10 +10844,38 @@
         <v>82</v>
       </c>
       <c r="D120" s="3"/>
-      <c r="L120" s="1"/>
-      <c r="O120" s="2"/>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M120" s="12">
+        <v>7286768129</v>
+      </c>
+      <c r="N120" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O120" s="3">
+        <f>M120/M110*100</f>
+        <v>47.840308057278861</v>
+      </c>
+      <c r="Q120" s="12">
+        <v>7883995543</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="S120" s="3">
+        <f>Q120/Q110*100</f>
+        <v>49.245557199954867</v>
+      </c>
+      <c r="U120" s="12">
+        <v>11824933324</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="W120" s="3">
+        <f>U120/U110*100</f>
+        <v>63.690416578462127</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B121" s="3">
         <v>173352799</v>
       </c>
@@ -10611,7 +10888,7 @@
       </c>
       <c r="L121" s="1"/>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B122" s="3">
         <v>63797978806</v>
       </c>
@@ -10620,8 +10897,23 @@
       </c>
       <c r="D122" s="3"/>
       <c r="L122" s="1"/>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N122" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O122" t="s">
+        <v>113</v>
+      </c>
+      <c r="P122" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>108</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B123" s="3">
         <v>54417398</v>
       </c>
@@ -10634,8 +10926,26 @@
       </c>
       <c r="E123" s="2"/>
       <c r="L123" s="1"/>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M123" t="s">
+        <v>78</v>
+      </c>
+      <c r="N123" s="12">
+        <v>15231440651</v>
+      </c>
+      <c r="O123" s="11">
+        <v>4270922</v>
+      </c>
+      <c r="P123" s="11">
+        <v>3845831</v>
+      </c>
+      <c r="Q123" s="12">
+        <v>10140918426</v>
+      </c>
+      <c r="R123" s="12">
+        <v>7286768129</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B124" s="3">
         <v>138274168189</v>
       </c>
@@ -10644,9 +10954,26 @@
       </c>
       <c r="D124" s="3"/>
       <c r="L124" s="1"/>
-      <c r="O124" s="2"/>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M124" t="s">
+        <v>96</v>
+      </c>
+      <c r="N124" s="12">
+        <v>16009556986</v>
+      </c>
+      <c r="O124" s="11">
+        <v>8838189</v>
+      </c>
+      <c r="P124" s="11">
+        <v>8243551</v>
+      </c>
+      <c r="Q124" s="12">
+        <v>10574451072</v>
+      </c>
+      <c r="R124" s="12">
+        <v>7883995543</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B125" s="3">
         <v>1046512.406308</v>
       </c>
@@ -10654,8 +10981,26 @@
         <v>87</v>
       </c>
       <c r="D125" s="3"/>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M125" t="s">
+        <v>99</v>
+      </c>
+      <c r="N125" s="12">
+        <v>18566267830</v>
+      </c>
+      <c r="O125" s="11">
+        <v>18145926</v>
+      </c>
+      <c r="P125" s="11">
+        <v>17122446</v>
+      </c>
+      <c r="Q125" s="12">
+        <v>14199910081</v>
+      </c>
+      <c r="R125" s="12">
+        <v>11824933324</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B126" s="3">
         <v>1046501.290952</v>
       </c>
@@ -10665,7 +11010,7 @@
       <c r="D126" s="3"/>
       <c r="L126" s="1"/>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B127" s="3">
         <v>1999052526813</v>
       </c>
@@ -10678,7 +11023,7 @@
       </c>
       <c r="L127" s="1"/>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B128" s="3">
         <v>1366120186531</v>
       </c>

</xml_diff>